<commit_message>
Add 27-mar and GLM predictions for different days
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD258F03-9E6F-0341-A836-FF439ADE0C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39815CF8-90A1-114A-9DA0-8960B6498A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -116,8 +116,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{37410649-CFF6-DD40-AA2D-A41F8321A833}" name="tabula-Actualizacion_57_COVID-19(1)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_57_COVID-19(1).csv" decimal="," thousands="." tab="0" comma="1">
+  <connection id="6" xr16:uid="{37410649-CFF6-DD40-AA2D-A41F8321A833}" name="tabula-Actualizacion_57_COVID-19(1)" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_57_COVID-19(1).csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -282,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -293,6 +293,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -312,27 +313,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -632,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,6 +651,14 @@
     <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.2">
@@ -4512,40 +4521,736 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="7"/>
-      <c r="H111" s="7"/>
-      <c r="J111" s="7"/>
+      <c r="A111" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>83</v>
+      </c>
+      <c r="E111">
+        <v>19</v>
+      </c>
+      <c r="F111">
+        <v>0.3</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D112" s="3"/>
-    </row>
-    <row r="113" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D113" s="3"/>
-    </row>
-    <row r="114" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-    </row>
-    <row r="115" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-    </row>
-    <row r="116" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-    </row>
-    <row r="117" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-    </row>
-    <row r="119" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="J119" s="7"/>
+      <c r="A112" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112">
+        <v>174</v>
+      </c>
+      <c r="E112">
+        <v>20</v>
+      </c>
+      <c r="F112">
+        <v>0.3</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>0.3</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>0.2</v>
+      </c>
+      <c r="K112">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1228</v>
+      </c>
+      <c r="E113">
+        <v>140</v>
+      </c>
+      <c r="F113">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G113">
+        <v>8</v>
+      </c>
+      <c r="H113">
+        <v>2.1</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2148</v>
+      </c>
+      <c r="E114">
+        <v>314</v>
+      </c>
+      <c r="F114">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G114">
+        <v>13</v>
+      </c>
+      <c r="H114">
+        <v>3.4</v>
+      </c>
+      <c r="I114">
+        <v>4</v>
+      </c>
+      <c r="J114">
+        <v>0.7</v>
+      </c>
+      <c r="K114">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" s="3">
+        <v>2973</v>
+      </c>
+      <c r="E115">
+        <v>580</v>
+      </c>
+      <c r="F115">
+        <v>9.4</v>
+      </c>
+      <c r="G115">
+        <v>32</v>
+      </c>
+      <c r="H115">
+        <v>8.4</v>
+      </c>
+      <c r="I115">
+        <v>10</v>
+      </c>
+      <c r="J115">
+        <v>1.8</v>
+      </c>
+      <c r="K115">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="3">
+        <v>3368</v>
+      </c>
+      <c r="E116">
+        <v>869</v>
+      </c>
+      <c r="F116">
+        <v>14</v>
+      </c>
+      <c r="G116">
+        <v>67</v>
+      </c>
+      <c r="H116">
+        <v>17.7</v>
+      </c>
+      <c r="I116">
+        <v>8</v>
+      </c>
+      <c r="J116">
+        <v>1.5</v>
+      </c>
+      <c r="K116">
+        <v>0.2</v>
+      </c>
+      <c r="M116" s="8"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="3">
+        <v>2790</v>
+      </c>
+      <c r="E117" s="3">
+        <v>1238</v>
+      </c>
+      <c r="F117">
+        <v>20</v>
+      </c>
+      <c r="G117">
+        <v>110</v>
+      </c>
+      <c r="H117">
+        <v>29</v>
+      </c>
+      <c r="I117">
+        <v>45</v>
+      </c>
+      <c r="J117">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K117">
+        <v>1.6</v>
+      </c>
+      <c r="N117" s="3"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="3">
+        <v>2396</v>
+      </c>
+      <c r="E118" s="3">
+        <v>1416</v>
+      </c>
+      <c r="F118">
+        <v>22.9</v>
+      </c>
+      <c r="G118">
+        <v>125</v>
+      </c>
+      <c r="H118">
+        <v>33</v>
+      </c>
+      <c r="I118">
+        <v>95</v>
+      </c>
+      <c r="J118">
+        <v>17.3</v>
+      </c>
+      <c r="K118">
+        <v>4</v>
+      </c>
+      <c r="N118" s="3"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="3">
+        <v>2076</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1181</v>
+      </c>
+      <c r="F119">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="G119">
+        <v>23</v>
+      </c>
+      <c r="H119">
+        <v>6.1</v>
+      </c>
+      <c r="I119">
+        <v>258</v>
+      </c>
+      <c r="J119">
+        <v>46.9</v>
+      </c>
+      <c r="K119">
+        <v>12.4</v>
+      </c>
+      <c r="N119" s="3"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120">
+        <v>891</v>
+      </c>
+      <c r="E120">
+        <v>416</v>
+      </c>
+      <c r="F120">
+        <v>6.7</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>129</v>
+      </c>
+      <c r="J120">
+        <v>23.5</v>
+      </c>
+      <c r="K120">
+        <v>14.5</v>
+      </c>
+      <c r="N120" s="3"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B121" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>103</v>
+      </c>
+      <c r="E121">
+        <v>30</v>
+      </c>
+      <c r="F121">
+        <v>0.3</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>0.1</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B122" t="s">
+        <v>10</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122">
+        <v>143</v>
+      </c>
+      <c r="E122">
+        <v>15</v>
+      </c>
+      <c r="F122">
+        <v>0.2</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B123" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>857</v>
+      </c>
+      <c r="E123">
+        <v>168</v>
+      </c>
+      <c r="F123">
+        <v>1.9</v>
+      </c>
+      <c r="G123">
+        <v>10</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <v>4</v>
+      </c>
+      <c r="J123">
+        <v>0.4</v>
+      </c>
+      <c r="K123">
+        <v>0.5</v>
+      </c>
+      <c r="N123" s="3"/>
+      <c r="O123" s="3"/>
+      <c r="P123" s="7"/>
+      <c r="R123" s="7"/>
+      <c r="T123" s="7"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" s="3">
+        <v>1626</v>
+      </c>
+      <c r="E124">
+        <v>383</v>
+      </c>
+      <c r="F124">
+        <v>4.3</v>
+      </c>
+      <c r="G124">
+        <v>28</v>
+      </c>
+      <c r="H124">
+        <v>2.9</v>
+      </c>
+      <c r="I124">
+        <v>3</v>
+      </c>
+      <c r="J124">
+        <v>0.3</v>
+      </c>
+      <c r="K124">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B125" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" t="s">
+        <v>3</v>
+      </c>
+      <c r="D125" s="3">
+        <v>2578</v>
+      </c>
+      <c r="E125">
+        <v>880</v>
+      </c>
+      <c r="F125">
+        <v>9.9</v>
+      </c>
+      <c r="G125">
+        <v>76</v>
+      </c>
+      <c r="H125">
+        <v>7.9</v>
+      </c>
+      <c r="I125">
+        <v>9</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B126" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126" s="3">
+        <v>3054</v>
+      </c>
+      <c r="E126" s="3">
+        <v>1331</v>
+      </c>
+      <c r="F126">
+        <v>15</v>
+      </c>
+      <c r="G126">
+        <v>159</v>
+      </c>
+      <c r="H126">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I126">
+        <v>29</v>
+      </c>
+      <c r="J126">
+        <v>3.3</v>
+      </c>
+      <c r="K126">
+        <v>0.9</v>
+      </c>
+      <c r="M126" s="8"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B127" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="3">
+        <v>3187</v>
+      </c>
+      <c r="E127" s="3">
+        <v>1760</v>
+      </c>
+      <c r="F127">
+        <v>19.8</v>
+      </c>
+      <c r="G127">
+        <v>282</v>
+      </c>
+      <c r="H127">
+        <v>29.4</v>
+      </c>
+      <c r="I127">
+        <v>78</v>
+      </c>
+      <c r="J127">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K127">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="3">
+        <v>3527</v>
+      </c>
+      <c r="E128" s="3">
+        <v>2372</v>
+      </c>
+      <c r="F128">
+        <v>26.7</v>
+      </c>
+      <c r="G128">
+        <v>365</v>
+      </c>
+      <c r="H128">
+        <v>38.1</v>
+      </c>
+      <c r="I128">
+        <v>248</v>
+      </c>
+      <c r="J128">
+        <v>27.8</v>
+      </c>
+      <c r="K128">
+        <v>7</v>
+      </c>
+      <c r="N128" s="3"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B129" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" s="3">
+        <v>2421</v>
+      </c>
+      <c r="E129" s="3">
+        <v>1610</v>
+      </c>
+      <c r="F129">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="G129">
+        <v>33</v>
+      </c>
+      <c r="H129">
+        <v>3.4</v>
+      </c>
+      <c r="I129">
+        <v>384</v>
+      </c>
+      <c r="J129">
+        <v>43</v>
+      </c>
+      <c r="K129">
+        <v>15.9</v>
+      </c>
+      <c r="N129" s="3"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B130" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130">
+        <v>574</v>
+      </c>
+      <c r="E130">
+        <v>350</v>
+      </c>
+      <c r="F130">
+        <v>3.9</v>
+      </c>
+      <c r="G130">
+        <v>5</v>
+      </c>
+      <c r="H130">
+        <v>0.5</v>
+      </c>
+      <c r="I130">
+        <v>137</v>
+      </c>
+      <c r="J130">
+        <v>15.4</v>
+      </c>
+      <c r="K130">
+        <v>23.9</v>
+      </c>
+      <c r="N130" s="3"/>
+      <c r="O130" s="3"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N131" s="3"/>
+      <c r="O131" s="3"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N132" s="3"/>
+      <c r="O132" s="3"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N134" s="3"/>
+      <c r="O134" s="3"/>
+      <c r="P134" s="7"/>
+      <c r="R134" s="7"/>
+      <c r="T134" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding 1-apr data for real
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5A423-41BA-D142-8D7C-E8CD8E9347DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD58EC5-7C98-D24A-9A50-A2AC4D9E5003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -28,6 +28,7 @@
     <definedName name="tabula_Actualizacion_61_COVID_19_1" localSheetId="0">Data!$C$171:$J$190</definedName>
     <definedName name="tabula_Actualizacion_61_COVID_19_2__1" localSheetId="0">Data!$C$171:$K$190</definedName>
     <definedName name="tabula_Actualizacion_62_COVID_19_1" localSheetId="0">Data!$C$191:$K$210</definedName>
+    <definedName name="tabula_Actualizacion_63_COVID_19_1" localSheetId="0">Data!$C$211:$K$230</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -196,7 +197,22 @@
     </textPr>
   </connection>
   <connection id="11" xr16:uid="{D9E753A3-0975-2B4A-A431-4575D72D0DD4}" name="tabula-Actualizacion_62_COVID-19(1)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_62_COVID-19(1).csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_62_COVID-19(1).csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" xr16:uid="{3D624737-D49D-F448-8970-DEE31EFF2B05}" name="tabula-Actualizacion_63_COVID-19(1)" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_63_COVID-19(1).csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -214,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -392,47 +408,51 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,21 +752,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:T211"/>
+  <dimension ref="A1:T230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="G210" sqref="G210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -8166,8 +8184,706 @@
       <c r="O210" s="3"/>
     </row>
     <row r="211" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B211" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211" t="s">
+        <v>0</v>
+      </c>
+      <c r="D211">
+        <v>116</v>
+      </c>
+      <c r="E211">
+        <v>36</v>
+      </c>
+      <c r="F211">
+        <v>0.3</v>
+      </c>
+      <c r="G211">
+        <v>2</v>
+      </c>
+      <c r="H211">
+        <v>0.3</v>
+      </c>
+      <c r="I211">
+        <v>1</v>
+      </c>
+      <c r="J211">
+        <v>0.1</v>
+      </c>
+      <c r="K211">
+        <v>0.9</v>
+      </c>
       <c r="N211" s="3"/>
       <c r="O211" s="3"/>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B212" t="s">
+        <v>9</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D212">
+        <v>223</v>
+      </c>
+      <c r="E212">
+        <v>39</v>
+      </c>
+      <c r="F212">
+        <v>0.3</v>
+      </c>
+      <c r="G212">
+        <v>1</v>
+      </c>
+      <c r="H212">
+        <v>0.1</v>
+      </c>
+      <c r="I212">
+        <v>1</v>
+      </c>
+      <c r="J212">
+        <v>0.1</v>
+      </c>
+      <c r="K212">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B213" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1</v>
+      </c>
+      <c r="D213" s="3">
+        <v>2233</v>
+      </c>
+      <c r="E213">
+        <v>270</v>
+      </c>
+      <c r="F213">
+        <v>2.1</v>
+      </c>
+      <c r="G213">
+        <v>11</v>
+      </c>
+      <c r="H213">
+        <v>1.5</v>
+      </c>
+      <c r="I213">
+        <v>1</v>
+      </c>
+      <c r="J213">
+        <v>0.1</v>
+      </c>
+      <c r="K213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B214" t="s">
+        <v>9</v>
+      </c>
+      <c r="C214" t="s">
+        <v>2</v>
+      </c>
+      <c r="D214" s="3">
+        <v>4028</v>
+      </c>
+      <c r="E214">
+        <v>642</v>
+      </c>
+      <c r="F214">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G214">
+        <v>30</v>
+      </c>
+      <c r="H214">
+        <v>4.2</v>
+      </c>
+      <c r="I214">
+        <v>7</v>
+      </c>
+      <c r="J214">
+        <v>0.4</v>
+      </c>
+      <c r="K214">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B215" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215" t="s">
+        <v>3</v>
+      </c>
+      <c r="D215" s="3">
+        <v>5731</v>
+      </c>
+      <c r="E215" s="3">
+        <v>1204</v>
+      </c>
+      <c r="F215">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G215">
+        <v>64</v>
+      </c>
+      <c r="H215">
+        <v>8.9</v>
+      </c>
+      <c r="I215">
+        <v>20</v>
+      </c>
+      <c r="J215">
+        <v>1.2</v>
+      </c>
+      <c r="K215">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B216" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" t="s">
+        <v>4</v>
+      </c>
+      <c r="D216" s="3">
+        <v>6740</v>
+      </c>
+      <c r="E216" s="3">
+        <v>1876</v>
+      </c>
+      <c r="F216">
+        <v>14.3</v>
+      </c>
+      <c r="G216">
+        <v>130</v>
+      </c>
+      <c r="H216">
+        <v>18</v>
+      </c>
+      <c r="I216">
+        <v>43</v>
+      </c>
+      <c r="J216">
+        <v>2.6</v>
+      </c>
+      <c r="K216">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B217" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217" t="s">
+        <v>5</v>
+      </c>
+      <c r="D217" s="3">
+        <v>5330</v>
+      </c>
+      <c r="E217" s="3">
+        <v>2559</v>
+      </c>
+      <c r="F217">
+        <v>19.5</v>
+      </c>
+      <c r="G217">
+        <v>209</v>
+      </c>
+      <c r="H217">
+        <v>28.9</v>
+      </c>
+      <c r="I217">
+        <v>111</v>
+      </c>
+      <c r="J217">
+        <v>6.7</v>
+      </c>
+      <c r="K217">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B218" t="s">
+        <v>9</v>
+      </c>
+      <c r="C218" t="s">
+        <v>6</v>
+      </c>
+      <c r="D218" s="3">
+        <v>4636</v>
+      </c>
+      <c r="E218" s="3">
+        <v>3078</v>
+      </c>
+      <c r="F218">
+        <v>23.5</v>
+      </c>
+      <c r="G218">
+        <v>222</v>
+      </c>
+      <c r="H218">
+        <v>30.7</v>
+      </c>
+      <c r="I218">
+        <v>333</v>
+      </c>
+      <c r="J218">
+        <v>20.2</v>
+      </c>
+      <c r="K218">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B219" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219" t="s">
+        <v>12</v>
+      </c>
+      <c r="D219" s="3">
+        <v>4279</v>
+      </c>
+      <c r="E219" s="3">
+        <v>2559</v>
+      </c>
+      <c r="F219">
+        <v>19.5</v>
+      </c>
+      <c r="G219">
+        <v>51</v>
+      </c>
+      <c r="H219">
+        <v>7.1</v>
+      </c>
+      <c r="I219">
+        <v>743</v>
+      </c>
+      <c r="J219">
+        <v>45.1</v>
+      </c>
+      <c r="K219">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B220" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" t="s">
+        <v>13</v>
+      </c>
+      <c r="D220" s="3">
+        <v>1775</v>
+      </c>
+      <c r="E220">
+        <v>848</v>
+      </c>
+      <c r="F220">
+        <v>6.5</v>
+      </c>
+      <c r="G220">
+        <v>2</v>
+      </c>
+      <c r="H220">
+        <v>0.3</v>
+      </c>
+      <c r="I220">
+        <v>389</v>
+      </c>
+      <c r="J220">
+        <v>23.6</v>
+      </c>
+      <c r="K220">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B221" t="s">
+        <v>10</v>
+      </c>
+      <c r="C221" t="s">
+        <v>0</v>
+      </c>
+      <c r="D221">
+        <v>135</v>
+      </c>
+      <c r="E221">
+        <v>50</v>
+      </c>
+      <c r="F221">
+        <v>0.3</v>
+      </c>
+      <c r="G221">
+        <v>5</v>
+      </c>
+      <c r="H221">
+        <v>0.3</v>
+      </c>
+      <c r="I221">
+        <v>0</v>
+      </c>
+      <c r="J221">
+        <v>0</v>
+      </c>
+      <c r="K221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B222" t="s">
+        <v>10</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D222">
+        <v>210</v>
+      </c>
+      <c r="E222">
+        <v>33</v>
+      </c>
+      <c r="F222">
+        <v>0.2</v>
+      </c>
+      <c r="G222">
+        <v>2</v>
+      </c>
+      <c r="H222">
+        <v>0.1</v>
+      </c>
+      <c r="I222">
+        <v>0</v>
+      </c>
+      <c r="J222">
+        <v>0</v>
+      </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B223" t="s">
+        <v>10</v>
+      </c>
+      <c r="C223" t="s">
+        <v>1</v>
+      </c>
+      <c r="D223" s="3">
+        <v>1356</v>
+      </c>
+      <c r="E223">
+        <v>274</v>
+      </c>
+      <c r="F223">
+        <v>1.4</v>
+      </c>
+      <c r="G223">
+        <v>18</v>
+      </c>
+      <c r="H223">
+        <v>1</v>
+      </c>
+      <c r="I223">
+        <v>5</v>
+      </c>
+      <c r="J223">
+        <v>0.2</v>
+      </c>
+      <c r="K223">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B224" t="s">
+        <v>10</v>
+      </c>
+      <c r="C224" t="s">
+        <v>2</v>
+      </c>
+      <c r="D224" s="3">
+        <v>2824</v>
+      </c>
+      <c r="E224">
+        <v>734</v>
+      </c>
+      <c r="F224">
+        <v>3.9</v>
+      </c>
+      <c r="G224">
+        <v>56</v>
+      </c>
+      <c r="H224">
+        <v>3.2</v>
+      </c>
+      <c r="I224">
+        <v>12</v>
+      </c>
+      <c r="J224">
+        <v>0.4</v>
+      </c>
+      <c r="K224">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B225" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225" t="s">
+        <v>3</v>
+      </c>
+      <c r="D225" s="3">
+        <v>4822</v>
+      </c>
+      <c r="E225" s="3">
+        <v>1833</v>
+      </c>
+      <c r="F225">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G225">
+        <v>150</v>
+      </c>
+      <c r="H225">
+        <v>8.5</v>
+      </c>
+      <c r="I225">
+        <v>32</v>
+      </c>
+      <c r="J225">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K225">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C226" t="s">
+        <v>4</v>
+      </c>
+      <c r="D226" s="3">
+        <v>5979</v>
+      </c>
+      <c r="E226" s="3">
+        <v>2918</v>
+      </c>
+      <c r="F226">
+        <v>15.4</v>
+      </c>
+      <c r="G226">
+        <v>301</v>
+      </c>
+      <c r="H226">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I226">
+        <v>94</v>
+      </c>
+      <c r="J226">
+        <v>3.3</v>
+      </c>
+      <c r="K226">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B227" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227" t="s">
+        <v>5</v>
+      </c>
+      <c r="D227" s="3">
+        <v>6320</v>
+      </c>
+      <c r="E227" s="3">
+        <v>3949</v>
+      </c>
+      <c r="F227">
+        <v>20.9</v>
+      </c>
+      <c r="G227">
+        <v>570</v>
+      </c>
+      <c r="H227">
+        <v>32.4</v>
+      </c>
+      <c r="I227">
+        <v>274</v>
+      </c>
+      <c r="J227">
+        <v>9.5</v>
+      </c>
+      <c r="K227">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B228" t="s">
+        <v>10</v>
+      </c>
+      <c r="C228" t="s">
+        <v>6</v>
+      </c>
+      <c r="D228" s="3">
+        <v>6727</v>
+      </c>
+      <c r="E228" s="3">
+        <v>5032</v>
+      </c>
+      <c r="F228">
+        <v>26.6</v>
+      </c>
+      <c r="G228">
+        <v>597</v>
+      </c>
+      <c r="H228">
+        <v>34</v>
+      </c>
+      <c r="I228">
+        <v>887</v>
+      </c>
+      <c r="J228">
+        <v>30.9</v>
+      </c>
+      <c r="K228">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B229" t="s">
+        <v>10</v>
+      </c>
+      <c r="C229" t="s">
+        <v>12</v>
+      </c>
+      <c r="D229" s="3">
+        <v>4577</v>
+      </c>
+      <c r="E229" s="3">
+        <v>3370</v>
+      </c>
+      <c r="F229">
+        <v>17.8</v>
+      </c>
+      <c r="G229">
+        <v>54</v>
+      </c>
+      <c r="H229">
+        <v>3.1</v>
+      </c>
+      <c r="I229">
+        <v>1205</v>
+      </c>
+      <c r="J229">
+        <v>41.9</v>
+      </c>
+      <c r="K229">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B230" t="s">
+        <v>10</v>
+      </c>
+      <c r="C230" t="s">
+        <v>13</v>
+      </c>
+      <c r="D230" s="3">
+        <v>1119</v>
+      </c>
+      <c r="E230">
+        <v>715</v>
+      </c>
+      <c r="F230">
+        <v>3.8</v>
+      </c>
+      <c r="G230">
+        <v>4</v>
+      </c>
+      <c r="H230">
+        <v>0.2</v>
+      </c>
+      <c r="I230">
+        <v>364</v>
+      </c>
+      <c r="J230">
+        <v>12.7</v>
+      </c>
+      <c r="K230">
+        <v>32.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing gender data and adding 14-apr data
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0AB7A-A479-2A40-9D84-A69B8AE570E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A463966-A672-6C41-A494-C1CE98AE9701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -41,6 +41,7 @@
     <definedName name="tabula_Actualizacion_73_COVID_19_1" localSheetId="0">Data!$C$411:$K$430</definedName>
     <definedName name="tabula_Actualizacion_74_COVID_19_1" localSheetId="0">Data!$C$431:$K$450</definedName>
     <definedName name="tabula_Actualizacion_75_COVID_19_1" localSheetId="0">Data!$C$451:$K$470</definedName>
+    <definedName name="tabula_Actualizacion_76_COVID_19_2" localSheetId="0">Data!$C$471:$K$490</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -404,7 +405,22 @@
     </textPr>
   </connection>
   <connection id="24" xr16:uid="{21D9C3D0-364D-7245-9386-57E3291626E2}" name="tabula-Actualizacion_75_COVID-19(1)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_75_COVID-19(1).csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_75_COVID-19(1).csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="25" xr16:uid="{AA55B43A-6669-3349-88E7-2C63E39C369C}" name="tabula-Actualizacion_76_COVID-19(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_76_COVID-19(2).csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -422,7 +438,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -600,7 +616,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -608,91 +624,95 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_65_COVID-19(1)" connectionId="14" xr16:uid="{1F7FC7F3-ADF7-CE4C-A901-C09AA03AA932}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -992,15 +1012,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:T470"/>
+  <dimension ref="A1:T490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
-      <selection activeCell="E451" sqref="E451"/>
+    <sheetView tabSelected="1" topLeftCell="A454" workbookViewId="0">
+      <selection activeCell="E476" sqref="E476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
@@ -16797,7 +16817,7 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B450" t="s">
         <v>10</v>
@@ -17528,6 +17548,706 @@
       </c>
       <c r="K470">
         <v>33.6</v>
+      </c>
+    </row>
+    <row r="471" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A471" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B471" t="s">
+        <v>9</v>
+      </c>
+      <c r="C471" t="s">
+        <v>0</v>
+      </c>
+      <c r="D471">
+        <v>177</v>
+      </c>
+      <c r="E471">
+        <v>57</v>
+      </c>
+      <c r="F471">
+        <v>0.2</v>
+      </c>
+      <c r="G471">
+        <v>1</v>
+      </c>
+      <c r="H471">
+        <v>0</v>
+      </c>
+      <c r="I471">
+        <v>1</v>
+      </c>
+      <c r="J471">
+        <v>0</v>
+      </c>
+      <c r="K471">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="472" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A472" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B472" t="s">
+        <v>9</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D472">
+        <v>361</v>
+      </c>
+      <c r="E472">
+        <v>73</v>
+      </c>
+      <c r="F472">
+        <v>0.3</v>
+      </c>
+      <c r="G472">
+        <v>2</v>
+      </c>
+      <c r="H472">
+        <v>0.1</v>
+      </c>
+      <c r="I472">
+        <v>1</v>
+      </c>
+      <c r="J472">
+        <v>0</v>
+      </c>
+      <c r="K472">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="473" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A473" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B473" t="s">
+        <v>9</v>
+      </c>
+      <c r="C473" t="s">
+        <v>1</v>
+      </c>
+      <c r="D473" s="3">
+        <v>4094</v>
+      </c>
+      <c r="E473">
+        <v>463</v>
+      </c>
+      <c r="F473">
+        <v>1.9</v>
+      </c>
+      <c r="G473">
+        <v>18</v>
+      </c>
+      <c r="H473">
+        <v>0.8</v>
+      </c>
+      <c r="I473">
+        <v>5</v>
+      </c>
+      <c r="J473">
+        <v>0.1</v>
+      </c>
+      <c r="K473">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A474" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B474" t="s">
+        <v>9</v>
+      </c>
+      <c r="C474" t="s">
+        <v>2</v>
+      </c>
+      <c r="D474" s="3">
+        <v>7125</v>
+      </c>
+      <c r="E474" s="3">
+        <v>1136</v>
+      </c>
+      <c r="F474">
+        <v>4.7</v>
+      </c>
+      <c r="G474">
+        <v>47</v>
+      </c>
+      <c r="H474">
+        <v>2</v>
+      </c>
+      <c r="I474">
+        <v>15</v>
+      </c>
+      <c r="J474">
+        <v>0.4</v>
+      </c>
+      <c r="K474">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="475" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A475" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B475" t="s">
+        <v>9</v>
+      </c>
+      <c r="C475" t="s">
+        <v>3</v>
+      </c>
+      <c r="D475" s="3">
+        <v>10236</v>
+      </c>
+      <c r="E475" s="3">
+        <v>2202</v>
+      </c>
+      <c r="F475">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G475">
+        <v>104</v>
+      </c>
+      <c r="H475">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I475">
+        <v>39</v>
+      </c>
+      <c r="J475">
+        <v>1</v>
+      </c>
+      <c r="K475">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="476" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A476" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B476" t="s">
+        <v>9</v>
+      </c>
+      <c r="C476" t="s">
+        <v>4</v>
+      </c>
+      <c r="D476" s="3">
+        <v>12409</v>
+      </c>
+      <c r="E476" s="3">
+        <v>3562</v>
+      </c>
+      <c r="F476">
+        <v>14.8</v>
+      </c>
+      <c r="G476">
+        <v>223</v>
+      </c>
+      <c r="H476">
+        <v>9.5</v>
+      </c>
+      <c r="I476">
+        <v>89</v>
+      </c>
+      <c r="J476">
+        <v>2.4</v>
+      </c>
+      <c r="K476">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A477" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B477" t="s">
+        <v>9</v>
+      </c>
+      <c r="C477" t="s">
+        <v>5</v>
+      </c>
+      <c r="D477" s="3">
+        <v>9332</v>
+      </c>
+      <c r="E477" s="3">
+        <v>4515</v>
+      </c>
+      <c r="F477">
+        <v>18.8</v>
+      </c>
+      <c r="G477">
+        <v>395</v>
+      </c>
+      <c r="H477">
+        <v>16.7</v>
+      </c>
+      <c r="I477">
+        <v>264</v>
+      </c>
+      <c r="J477">
+        <v>7</v>
+      </c>
+      <c r="K477">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A478" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B478" t="s">
+        <v>9</v>
+      </c>
+      <c r="C478" t="s">
+        <v>6</v>
+      </c>
+      <c r="D478" s="3">
+        <v>8069</v>
+      </c>
+      <c r="E478" s="3">
+        <v>5434</v>
+      </c>
+      <c r="F478">
+        <v>22.6</v>
+      </c>
+      <c r="G478">
+        <v>667</v>
+      </c>
+      <c r="H478">
+        <v>28.3</v>
+      </c>
+      <c r="I478">
+        <v>778</v>
+      </c>
+      <c r="J478">
+        <v>20.8</v>
+      </c>
+      <c r="K478">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A479" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B479" t="s">
+        <v>9</v>
+      </c>
+      <c r="C479" t="s">
+        <v>12</v>
+      </c>
+      <c r="D479" s="3">
+        <v>8830</v>
+      </c>
+      <c r="E479" s="3">
+        <v>4938</v>
+      </c>
+      <c r="F479">
+        <v>20.6</v>
+      </c>
+      <c r="G479">
+        <v>647</v>
+      </c>
+      <c r="H479">
+        <v>27.4</v>
+      </c>
+      <c r="I479" s="3">
+        <v>1653</v>
+      </c>
+      <c r="J479">
+        <v>44.1</v>
+      </c>
+      <c r="K479">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="480" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A480" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B480" t="s">
+        <v>9</v>
+      </c>
+      <c r="C480" t="s">
+        <v>13</v>
+      </c>
+      <c r="D480" s="3">
+        <v>4144</v>
+      </c>
+      <c r="E480" s="3">
+        <v>1646</v>
+      </c>
+      <c r="F480">
+        <v>6.9</v>
+      </c>
+      <c r="G480">
+        <v>255</v>
+      </c>
+      <c r="H480">
+        <v>10.8</v>
+      </c>
+      <c r="I480">
+        <v>901</v>
+      </c>
+      <c r="J480">
+        <v>24.1</v>
+      </c>
+      <c r="K480">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="481" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A481" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B481" t="s">
+        <v>10</v>
+      </c>
+      <c r="C481" t="s">
+        <v>0</v>
+      </c>
+      <c r="D481">
+        <v>205</v>
+      </c>
+      <c r="E481">
+        <v>80</v>
+      </c>
+      <c r="F481">
+        <v>0.2</v>
+      </c>
+      <c r="G481">
+        <v>14</v>
+      </c>
+      <c r="H481">
+        <v>0.4</v>
+      </c>
+      <c r="I481">
+        <v>0</v>
+      </c>
+      <c r="J481">
+        <v>0</v>
+      </c>
+      <c r="K481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A482" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B482" t="s">
+        <v>10</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D482">
+        <v>321</v>
+      </c>
+      <c r="E482">
+        <v>59</v>
+      </c>
+      <c r="F482">
+        <v>0.2</v>
+      </c>
+      <c r="G482">
+        <v>4</v>
+      </c>
+      <c r="H482">
+        <v>0.1</v>
+      </c>
+      <c r="I482">
+        <v>0</v>
+      </c>
+      <c r="J482">
+        <v>0</v>
+      </c>
+      <c r="K482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A483" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B483" t="s">
+        <v>10</v>
+      </c>
+      <c r="C483" t="s">
+        <v>1</v>
+      </c>
+      <c r="D483" s="3">
+        <v>2192</v>
+      </c>
+      <c r="E483">
+        <v>448</v>
+      </c>
+      <c r="F483">
+        <v>1.4</v>
+      </c>
+      <c r="G483">
+        <v>32</v>
+      </c>
+      <c r="H483">
+        <v>0.9</v>
+      </c>
+      <c r="I483">
+        <v>12</v>
+      </c>
+      <c r="J483">
+        <v>0.2</v>
+      </c>
+      <c r="K483">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A484" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B484" t="s">
+        <v>10</v>
+      </c>
+      <c r="C484" t="s">
+        <v>2</v>
+      </c>
+      <c r="D484" s="3">
+        <v>4626</v>
+      </c>
+      <c r="E484" s="3">
+        <v>1279</v>
+      </c>
+      <c r="F484">
+        <v>3.9</v>
+      </c>
+      <c r="G484">
+        <v>107</v>
+      </c>
+      <c r="H484">
+        <v>3.1</v>
+      </c>
+      <c r="I484">
+        <v>21</v>
+      </c>
+      <c r="J484">
+        <v>0.4</v>
+      </c>
+      <c r="K484">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A485" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B485" t="s">
+        <v>10</v>
+      </c>
+      <c r="C485" t="s">
+        <v>3</v>
+      </c>
+      <c r="D485" s="3">
+        <v>8149</v>
+      </c>
+      <c r="E485" s="3">
+        <v>3312</v>
+      </c>
+      <c r="F485">
+        <v>10</v>
+      </c>
+      <c r="G485">
+        <v>309</v>
+      </c>
+      <c r="H485">
+        <v>9</v>
+      </c>
+      <c r="I485">
+        <v>74</v>
+      </c>
+      <c r="J485">
+        <v>1.3</v>
+      </c>
+      <c r="K485">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="486" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A486" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B486" t="s">
+        <v>10</v>
+      </c>
+      <c r="C486" t="s">
+        <v>4</v>
+      </c>
+      <c r="D486" s="3">
+        <v>10432</v>
+      </c>
+      <c r="E486" s="3">
+        <v>5401</v>
+      </c>
+      <c r="F486">
+        <v>16.3</v>
+      </c>
+      <c r="G486">
+        <v>682</v>
+      </c>
+      <c r="H486">
+        <v>19.8</v>
+      </c>
+      <c r="I486">
+        <v>195</v>
+      </c>
+      <c r="J486">
+        <v>3.4</v>
+      </c>
+      <c r="K486">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A487" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B487" t="s">
+        <v>10</v>
+      </c>
+      <c r="C487" t="s">
+        <v>5</v>
+      </c>
+      <c r="D487" s="3">
+        <v>10802</v>
+      </c>
+      <c r="E487" s="3">
+        <v>6991</v>
+      </c>
+      <c r="F487">
+        <v>21.1</v>
+      </c>
+      <c r="G487" s="3">
+        <v>1132</v>
+      </c>
+      <c r="H487">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I487">
+        <v>644</v>
+      </c>
+      <c r="J487">
+        <v>11.2</v>
+      </c>
+      <c r="K487">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A488" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B488" t="s">
+        <v>10</v>
+      </c>
+      <c r="C488" t="s">
+        <v>6</v>
+      </c>
+      <c r="D488" s="3">
+        <v>10970</v>
+      </c>
+      <c r="E488" s="3">
+        <v>8328</v>
+      </c>
+      <c r="F488">
+        <v>25.2</v>
+      </c>
+      <c r="G488" s="3">
+        <v>1070</v>
+      </c>
+      <c r="H488">
+        <v>31.1</v>
+      </c>
+      <c r="I488" s="3">
+        <v>1842</v>
+      </c>
+      <c r="J488">
+        <v>31.9</v>
+      </c>
+      <c r="K488">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="489" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A489" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B489" t="s">
+        <v>10</v>
+      </c>
+      <c r="C489" t="s">
+        <v>12</v>
+      </c>
+      <c r="D489" s="3">
+        <v>8132</v>
+      </c>
+      <c r="E489" s="3">
+        <v>5886</v>
+      </c>
+      <c r="F489">
+        <v>17.8</v>
+      </c>
+      <c r="G489">
+        <v>87</v>
+      </c>
+      <c r="H489">
+        <v>2.5</v>
+      </c>
+      <c r="I489" s="3">
+        <v>2291</v>
+      </c>
+      <c r="J489">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="K489">
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A490" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B490" t="s">
+        <v>10</v>
+      </c>
+      <c r="C490" t="s">
+        <v>13</v>
+      </c>
+      <c r="D490" s="3">
+        <v>2191</v>
+      </c>
+      <c r="E490" s="3">
+        <v>1282</v>
+      </c>
+      <c r="F490">
+        <v>3.9</v>
+      </c>
+      <c r="G490">
+        <v>9</v>
+      </c>
+      <c r="H490">
+        <v>0.3</v>
+      </c>
+      <c r="I490">
+        <v>695</v>
+      </c>
+      <c r="J490">
+        <v>12</v>
+      </c>
+      <c r="K490">
+        <v>31.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding 16-apr and removing recovered from daily graph
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832AACF-BF29-4E49-82F3-127799A6F6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C710480C-F086-E144-86E6-25F9F9482B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -43,6 +43,7 @@
     <definedName name="tabula_Actualizacion_75_COVID_19_1" localSheetId="0">Data!$C$451:$K$470</definedName>
     <definedName name="tabula_Actualizacion_76_COVID_19_2" localSheetId="0">Data!$C$471:$K$490</definedName>
     <definedName name="tabula_Actualizacion_77_COVID_19_2" localSheetId="0">Data!$C$491:$K$510</definedName>
+    <definedName name="tabula_Actualizacion_78_COVID_19_2" localSheetId="0">Data!$C$511:$K$530</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -436,7 +437,22 @@
     </textPr>
   </connection>
   <connection id="26" xr16:uid="{31DBD363-9AEB-E24E-9EA5-B2B5E91D4C2B}" name="tabula-Actualizacion_77_COVID-19(2)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_77_COVID-19(2).csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_77_COVID-19(2).csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="27" xr16:uid="{DFC57172-597A-AC48-B3E6-DD954170BB9B}" name="tabula-Actualizacion_78_COVID-19(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_78_COVID-19(2).csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -454,7 +470,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -632,107 +648,111 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_78_COVID-19(2)" connectionId="27" xr16:uid="{DA1E7C1F-5CE0-764E-9BAE-85540697E15C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_77_COVID-19(2)" connectionId="26" xr16:uid="{B46FF584-84EC-AE4D-BCE8-171BFEBEEDEE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_65_COVID-19(1)" connectionId="14" xr16:uid="{1F7FC7F3-ADF7-CE4C-A901-C09AA03AA932}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_65_COVID-19(1)" connectionId="14" xr16:uid="{1F7FC7F3-ADF7-CE4C-A901-C09AA03AA932}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1032,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:T510"/>
+  <dimension ref="A1:T530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
-      <selection activeCell="Q496" sqref="Q496"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="C511" sqref="C511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18970,6 +18990,706 @@
         <v>31.5</v>
       </c>
     </row>
+    <row r="511" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A511" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B511" t="s">
+        <v>9</v>
+      </c>
+      <c r="C511" t="s">
+        <v>0</v>
+      </c>
+      <c r="D511">
+        <v>199</v>
+      </c>
+      <c r="E511">
+        <v>66</v>
+      </c>
+      <c r="F511">
+        <v>0.3</v>
+      </c>
+      <c r="G511">
+        <v>1</v>
+      </c>
+      <c r="H511">
+        <v>0</v>
+      </c>
+      <c r="I511">
+        <v>1</v>
+      </c>
+      <c r="J511">
+        <v>0</v>
+      </c>
+      <c r="K511">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="512" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A512" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B512" t="s">
+        <v>9</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D512">
+        <v>395</v>
+      </c>
+      <c r="E512">
+        <v>80</v>
+      </c>
+      <c r="F512">
+        <v>0.3</v>
+      </c>
+      <c r="G512">
+        <v>3</v>
+      </c>
+      <c r="H512">
+        <v>0.1</v>
+      </c>
+      <c r="I512">
+        <v>1</v>
+      </c>
+      <c r="J512">
+        <v>0</v>
+      </c>
+      <c r="K512">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="513" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A513" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B513" t="s">
+        <v>9</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1</v>
+      </c>
+      <c r="D513" s="3">
+        <v>4501</v>
+      </c>
+      <c r="E513">
+        <v>490</v>
+      </c>
+      <c r="F513">
+        <v>1.9</v>
+      </c>
+      <c r="G513">
+        <v>19</v>
+      </c>
+      <c r="H513">
+        <v>0.8</v>
+      </c>
+      <c r="I513">
+        <v>5</v>
+      </c>
+      <c r="J513">
+        <v>0.1</v>
+      </c>
+      <c r="K513">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A514" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B514" t="s">
+        <v>9</v>
+      </c>
+      <c r="C514" t="s">
+        <v>2</v>
+      </c>
+      <c r="D514" s="3">
+        <v>7764</v>
+      </c>
+      <c r="E514" s="3">
+        <v>1195</v>
+      </c>
+      <c r="F514">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G514">
+        <v>49</v>
+      </c>
+      <c r="H514">
+        <v>2</v>
+      </c>
+      <c r="I514">
+        <v>15</v>
+      </c>
+      <c r="J514">
+        <v>0.3</v>
+      </c>
+      <c r="K514">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="515" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A515" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B515" t="s">
+        <v>9</v>
+      </c>
+      <c r="C515" t="s">
+        <v>3</v>
+      </c>
+      <c r="D515" s="3">
+        <v>11221</v>
+      </c>
+      <c r="E515" s="3">
+        <v>2341</v>
+      </c>
+      <c r="F515">
+        <v>9</v>
+      </c>
+      <c r="G515">
+        <v>117</v>
+      </c>
+      <c r="H515">
+        <v>4.8</v>
+      </c>
+      <c r="I515">
+        <v>42</v>
+      </c>
+      <c r="J515">
+        <v>0.9</v>
+      </c>
+      <c r="K515">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="516" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A516" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B516" t="s">
+        <v>9</v>
+      </c>
+      <c r="C516" t="s">
+        <v>4</v>
+      </c>
+      <c r="D516" s="3">
+        <v>13684</v>
+      </c>
+      <c r="E516" s="3">
+        <v>3810</v>
+      </c>
+      <c r="F516">
+        <v>14.7</v>
+      </c>
+      <c r="G516">
+        <v>243</v>
+      </c>
+      <c r="H516">
+        <v>9.9</v>
+      </c>
+      <c r="I516">
+        <v>103</v>
+      </c>
+      <c r="J516">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K516">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="517" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A517" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B517" t="s">
+        <v>9</v>
+      </c>
+      <c r="C517" t="s">
+        <v>5</v>
+      </c>
+      <c r="D517" s="3">
+        <v>10037</v>
+      </c>
+      <c r="E517" s="3">
+        <v>4767</v>
+      </c>
+      <c r="F517">
+        <v>18.3</v>
+      </c>
+      <c r="G517">
+        <v>421</v>
+      </c>
+      <c r="H517">
+        <v>17.2</v>
+      </c>
+      <c r="I517">
+        <v>285</v>
+      </c>
+      <c r="J517">
+        <v>6.4</v>
+      </c>
+      <c r="K517">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="518" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A518" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B518" t="s">
+        <v>9</v>
+      </c>
+      <c r="C518" t="s">
+        <v>6</v>
+      </c>
+      <c r="D518" s="3">
+        <v>8847</v>
+      </c>
+      <c r="E518" s="3">
+        <v>5781</v>
+      </c>
+      <c r="F518">
+        <v>22.3</v>
+      </c>
+      <c r="G518">
+        <v>695</v>
+      </c>
+      <c r="H518">
+        <v>28.3</v>
+      </c>
+      <c r="I518">
+        <v>864</v>
+      </c>
+      <c r="J518">
+        <v>19.5</v>
+      </c>
+      <c r="K518">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="519" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A519" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B519" t="s">
+        <v>9</v>
+      </c>
+      <c r="C519" t="s">
+        <v>12</v>
+      </c>
+      <c r="D519" s="3">
+        <v>10685</v>
+      </c>
+      <c r="E519" s="3">
+        <v>5507</v>
+      </c>
+      <c r="F519">
+        <v>21.2</v>
+      </c>
+      <c r="G519">
+        <v>650</v>
+      </c>
+      <c r="H519">
+        <v>26.5</v>
+      </c>
+      <c r="I519" s="3">
+        <v>1961</v>
+      </c>
+      <c r="J519">
+        <v>44.3</v>
+      </c>
+      <c r="K519">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="520" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A520" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B520" t="s">
+        <v>9</v>
+      </c>
+      <c r="C520" t="s">
+        <v>13</v>
+      </c>
+      <c r="D520" s="3">
+        <v>5467</v>
+      </c>
+      <c r="E520" s="3">
+        <v>1944</v>
+      </c>
+      <c r="F520">
+        <v>7.5</v>
+      </c>
+      <c r="G520">
+        <v>256</v>
+      </c>
+      <c r="H520">
+        <v>10.4</v>
+      </c>
+      <c r="I520" s="3">
+        <v>1149</v>
+      </c>
+      <c r="J520">
+        <v>26</v>
+      </c>
+      <c r="K520">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="521" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A521" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B521" t="s">
+        <v>10</v>
+      </c>
+      <c r="C521" t="s">
+        <v>0</v>
+      </c>
+      <c r="D521">
+        <v>236</v>
+      </c>
+      <c r="E521">
+        <v>93</v>
+      </c>
+      <c r="F521">
+        <v>0.3</v>
+      </c>
+      <c r="G521">
+        <v>13</v>
+      </c>
+      <c r="H521">
+        <v>0.4</v>
+      </c>
+      <c r="I521">
+        <v>0</v>
+      </c>
+      <c r="J521">
+        <v>0</v>
+      </c>
+      <c r="K521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A522" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B522" t="s">
+        <v>10</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D522">
+        <v>345</v>
+      </c>
+      <c r="E522">
+        <v>70</v>
+      </c>
+      <c r="F522">
+        <v>0.2</v>
+      </c>
+      <c r="G522">
+        <v>5</v>
+      </c>
+      <c r="H522">
+        <v>0.1</v>
+      </c>
+      <c r="I522">
+        <v>1</v>
+      </c>
+      <c r="J522">
+        <v>0</v>
+      </c>
+      <c r="K522">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="523" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A523" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B523" t="s">
+        <v>10</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1</v>
+      </c>
+      <c r="D523" s="3">
+        <v>2360</v>
+      </c>
+      <c r="E523">
+        <v>479</v>
+      </c>
+      <c r="F523">
+        <v>1.4</v>
+      </c>
+      <c r="G523">
+        <v>32</v>
+      </c>
+      <c r="H523">
+        <v>0.9</v>
+      </c>
+      <c r="I523">
+        <v>15</v>
+      </c>
+      <c r="J523">
+        <v>0.2</v>
+      </c>
+      <c r="K523">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="524" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A524" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B524" t="s">
+        <v>10</v>
+      </c>
+      <c r="C524" t="s">
+        <v>2</v>
+      </c>
+      <c r="D524" s="3">
+        <v>4903</v>
+      </c>
+      <c r="E524" s="3">
+        <v>1337</v>
+      </c>
+      <c r="F524">
+        <v>3.8</v>
+      </c>
+      <c r="G524">
+        <v>114</v>
+      </c>
+      <c r="H524">
+        <v>3.1</v>
+      </c>
+      <c r="I524">
+        <v>22</v>
+      </c>
+      <c r="J524">
+        <v>0.3</v>
+      </c>
+      <c r="K524">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="525" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A525" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B525" t="s">
+        <v>10</v>
+      </c>
+      <c r="C525" t="s">
+        <v>3</v>
+      </c>
+      <c r="D525" s="3">
+        <v>8660</v>
+      </c>
+      <c r="E525" s="3">
+        <v>3481</v>
+      </c>
+      <c r="F525">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G525">
+        <v>324</v>
+      </c>
+      <c r="H525">
+        <v>8.9</v>
+      </c>
+      <c r="I525">
+        <v>76</v>
+      </c>
+      <c r="J525">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K525">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="526" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A526" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B526" t="s">
+        <v>10</v>
+      </c>
+      <c r="C526" t="s">
+        <v>4</v>
+      </c>
+      <c r="D526" s="3">
+        <v>11198</v>
+      </c>
+      <c r="E526" s="3">
+        <v>5728</v>
+      </c>
+      <c r="F526">
+        <v>16.2</v>
+      </c>
+      <c r="G526">
+        <v>726</v>
+      </c>
+      <c r="H526">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="I526">
+        <v>216</v>
+      </c>
+      <c r="J526">
+        <v>3.3</v>
+      </c>
+      <c r="K526">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="527" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A527" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B527" t="s">
+        <v>10</v>
+      </c>
+      <c r="C527" t="s">
+        <v>5</v>
+      </c>
+      <c r="D527" s="3">
+        <v>11562</v>
+      </c>
+      <c r="E527" s="3">
+        <v>7447</v>
+      </c>
+      <c r="F527">
+        <v>21</v>
+      </c>
+      <c r="G527" s="3">
+        <v>1218</v>
+      </c>
+      <c r="H527">
+        <v>33.4</v>
+      </c>
+      <c r="I527">
+        <v>687</v>
+      </c>
+      <c r="J527">
+        <v>10.3</v>
+      </c>
+      <c r="K527">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="528" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A528" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B528" t="s">
+        <v>10</v>
+      </c>
+      <c r="C528" t="s">
+        <v>6</v>
+      </c>
+      <c r="D528" s="3">
+        <v>11810</v>
+      </c>
+      <c r="E528" s="3">
+        <v>8845</v>
+      </c>
+      <c r="F528">
+        <v>25</v>
+      </c>
+      <c r="G528" s="3">
+        <v>1109</v>
+      </c>
+      <c r="H528">
+        <v>30.4</v>
+      </c>
+      <c r="I528" s="3">
+        <v>2062</v>
+      </c>
+      <c r="J528">
+        <v>31.1</v>
+      </c>
+      <c r="K528">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="529" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A529" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B529" t="s">
+        <v>10</v>
+      </c>
+      <c r="C529" t="s">
+        <v>12</v>
+      </c>
+      <c r="D529" s="3">
+        <v>9241</v>
+      </c>
+      <c r="E529" s="3">
+        <v>6447</v>
+      </c>
+      <c r="F529">
+        <v>18.2</v>
+      </c>
+      <c r="G529">
+        <v>95</v>
+      </c>
+      <c r="H529">
+        <v>2.6</v>
+      </c>
+      <c r="I529" s="3">
+        <v>2698</v>
+      </c>
+      <c r="J529">
+        <v>40.6</v>
+      </c>
+      <c r="K529">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="530" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A530" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B530" t="s">
+        <v>10</v>
+      </c>
+      <c r="C530" t="s">
+        <v>13</v>
+      </c>
+      <c r="D530" s="3">
+        <v>2667</v>
+      </c>
+      <c r="E530" s="3">
+        <v>1461</v>
+      </c>
+      <c r="F530">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G530">
+        <v>9</v>
+      </c>
+      <c r="H530">
+        <v>0.2</v>
+      </c>
+      <c r="I530">
+        <v>862</v>
+      </c>
+      <c r="J530">
+        <v>13</v>
+      </c>
+      <c r="K530">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding sexage data and limitation to 20 days in graph
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5B4984-CD06-E44F-BE4E-F051131CEB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6DCA5-BCF7-DB48-B4B1-3369AE7F866D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -54,6 +54,12 @@
     <definedName name="tabula_Actualizacion_86_COVID_19_2" localSheetId="0">Data!$C$671:$K$690</definedName>
     <definedName name="tabula_Actualizacion_87_COVID_19_2" localSheetId="0">Data!$C$691:$K$710</definedName>
     <definedName name="tabula_Actualizacion_88_COVID_19_2" localSheetId="0">Data!$C$711:$K$730</definedName>
+    <definedName name="tabula_Actualizacion_89_COVID_19" localSheetId="0">Data!$C$731:$K$750</definedName>
+    <definedName name="tabula_Actualizacion_90_COVID_19" localSheetId="0">Data!$C$751:$K$770</definedName>
+    <definedName name="tabula_Actualizacion_91_COVID_19" localSheetId="0">Data!$C$771:$K$790</definedName>
+    <definedName name="tabula_Actualizacion_92_COVID_19" localSheetId="0">Data!$C$791:$K$810</definedName>
+    <definedName name="tabula_Actualizacion_93_COVID_19" localSheetId="0">Data!$C$811:$K$830</definedName>
+    <definedName name="tabula_Actualizacion_94_COVID_19" localSheetId="0">Data!$C$831:$K$850</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -597,7 +603,7 @@
     </textPr>
   </connection>
   <connection id="36" xr16:uid="{73CF007A-6862-C443-8258-A45A2ABFA00D}" name="tabula-Actualizacion_87_COVID-19(2)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_87_COVID-19(2).csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_87_COVID-19(2).csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -612,7 +618,97 @@
     </textPr>
   </connection>
   <connection id="37" xr16:uid="{E8C1FC3E-CA51-6A46-B353-160355F9DC22}" name="tabula-Actualizacion_88_COVID-19(2)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_88_COVID-19(2).csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_88_COVID-19(2).csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="38" xr16:uid="{C3E1A69F-8B7E-6B43-BC5D-E06982B30200}" name="tabula-Actualizacion_89_COVID-191" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_89_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="39" xr16:uid="{087DFE1B-3741-FE4C-9B0D-327F1CED87AC}" name="tabula-Actualizacion_90_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_90_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="40" xr16:uid="{73C49DD9-FD9B-E141-A3F9-FED657D452BB}" name="tabula-Actualizacion_91_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_91_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="41" xr16:uid="{976AE8FA-AD7F-D745-A59B-524FC52002A8}" name="tabula-Actualizacion_92_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_92_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="42" xr16:uid="{D302820C-066C-364B-BDBB-65072DCE5142}" name="tabula-Actualizacion_93_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_93_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="43" xr16:uid="{7D726A8B-9669-2243-9E73-5A200DDE1F7F}" name="tabula-Actualizacion_94_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_94_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -630,7 +726,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -808,67 +904,67 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_88_COVID-19(2)" connectionId="37" xr16:uid="{442A7796-311C-914C-842C-C67D04E6CDF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_94_COVID-19" connectionId="43" xr16:uid="{E1DB3760-CEAD-1243-B89B-5083F9C5FD9D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_80_COVID-19(2)" connectionId="29" xr16:uid="{9A2F5700-61ED-F044-A56E-7B5EC6DF1036}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_87_COVID-19(2)" connectionId="36" xr16:uid="{3DC9730C-EB61-3546-A484-563DA03EF996}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_84_COVID-19(2)" connectionId="33" xr16:uid="{658D76C0-0942-AF43-952E-435C4A2BDAC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_65_COVID-19(1)" connectionId="14" xr16:uid="{1F7FC7F3-ADF7-CE4C-A901-C09AA03AA932}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_79_COVID-19(2)" connectionId="28" xr16:uid="{CE4041F5-2CDB-234C-8611-179139CF531A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_93_COVID-19" connectionId="42" xr16:uid="{9B502165-113E-5343-9630-B2499685DBE0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_77_COVID-19(2)" connectionId="26" xr16:uid="{B46FF584-84EC-AE4D-BCE8-171BFEBEEDEE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_84_COVID-19(2)" connectionId="33" xr16:uid="{658D76C0-0942-AF43-952E-435C4A2BDAC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_87_COVID-19(2)" connectionId="36" xr16:uid="{3DC9730C-EB61-3546-A484-563DA03EF996}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_65_COVID-19(1)" connectionId="14" xr16:uid="{1F7FC7F3-ADF7-CE4C-A901-C09AA03AA932}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_85_COVID-19(2)" connectionId="34" xr16:uid="{4236AA15-44DD-864C-BBB9-D1CF1013BE00}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_86_COVID-19(2)" connectionId="35" xr16:uid="{95015227-8A0A-4C48-AC40-AEF4A2B2143A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -876,83 +972,107 @@
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_92_COVID-19" connectionId="41" xr16:uid="{36511222-D462-6C49-8765-A7C39A844257}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_83_COVID-19(2)" connectionId="32" xr16:uid="{F68CD602-B2A0-604F-A4DC-A153B85916C5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_81_COVID-19(2)_1" connectionId="30" xr16:uid="{6EBD5E78-C6DF-2E41-9BEC-F2E99D2C6A50}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_80_COVID-19(2)" connectionId="29" xr16:uid="{9A2F5700-61ED-F044-A56E-7B5EC6DF1036}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_77_COVID-19(2)" connectionId="26" xr16:uid="{B46FF584-84EC-AE4D-BCE8-171BFEBEEDEE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_91_COVID-19" connectionId="40" xr16:uid="{84536095-CC54-8C41-83F7-F36B6B61C343}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_78_COVID-19(2)" connectionId="27" xr16:uid="{DA1E7C1F-5CE0-764E-9BAE-85540697E15C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_79_COVID-19(2)" connectionId="28" xr16:uid="{CE4041F5-2CDB-234C-8611-179139CF531A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_85_COVID-19(2)" connectionId="34" xr16:uid="{4236AA15-44DD-864C-BBB9-D1CF1013BE00}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_81_COVID-19(2)_1" connectionId="30" xr16:uid="{6EBD5E78-C6DF-2E41-9BEC-F2E99D2C6A50}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_78_COVID-19(2)" connectionId="27" xr16:uid="{DA1E7C1F-5CE0-764E-9BAE-85540697E15C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_90_COVID-19" connectionId="39" xr16:uid="{A93A93AC-3885-8E4E-8C26-49BA468F1F08}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_89_COVID-19" connectionId="38" xr16:uid="{7196C996-97E2-574F-AA83-DA40EB48943E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_88_COVID-19(2)" connectionId="37" xr16:uid="{442A7796-311C-914C-842C-C67D04E6CDF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_86_COVID-19(2)" connectionId="35" xr16:uid="{95015227-8A0A-4C48-AC40-AEF4A2B2143A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_83_COVID-19(2)" connectionId="32" xr16:uid="{F68CD602-B2A0-604F-A4DC-A153B85916C5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1252,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:T730"/>
+  <dimension ref="A1:T850"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A692" workbookViewId="0">
-      <selection activeCell="D715" sqref="D715"/>
+    <sheetView tabSelected="1" topLeftCell="A814" workbookViewId="0">
+      <selection activeCell="C842" sqref="C842"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26889,6 +27009,4206 @@
         <v>29.1</v>
       </c>
     </row>
+    <row r="731" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A731" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B731" t="s">
+        <v>9</v>
+      </c>
+      <c r="C731" t="s">
+        <v>0</v>
+      </c>
+      <c r="D731">
+        <v>304</v>
+      </c>
+      <c r="E731">
+        <v>99</v>
+      </c>
+      <c r="F731">
+        <v>0.3</v>
+      </c>
+      <c r="G731">
+        <v>11</v>
+      </c>
+      <c r="H731">
+        <v>0.5</v>
+      </c>
+      <c r="I731">
+        <v>1</v>
+      </c>
+      <c r="J731">
+        <v>0</v>
+      </c>
+      <c r="K731">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="732" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A732" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B732" t="s">
+        <v>9</v>
+      </c>
+      <c r="C732" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D732">
+        <v>668</v>
+      </c>
+      <c r="E732">
+        <v>121</v>
+      </c>
+      <c r="F732">
+        <v>0.3</v>
+      </c>
+      <c r="G732">
+        <v>8</v>
+      </c>
+      <c r="H732">
+        <v>0.4</v>
+      </c>
+      <c r="I732">
+        <v>3</v>
+      </c>
+      <c r="J732">
+        <v>0</v>
+      </c>
+      <c r="K732">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="733" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A733" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B733" t="s">
+        <v>9</v>
+      </c>
+      <c r="C733" t="s">
+        <v>1</v>
+      </c>
+      <c r="D733" s="3">
+        <v>7437</v>
+      </c>
+      <c r="E733">
+        <v>696</v>
+      </c>
+      <c r="F733">
+        <v>1.9</v>
+      </c>
+      <c r="G733">
+        <v>38</v>
+      </c>
+      <c r="H733">
+        <v>1.7</v>
+      </c>
+      <c r="I733">
+        <v>8</v>
+      </c>
+      <c r="J733">
+        <v>0.1</v>
+      </c>
+      <c r="K733">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="734" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A734" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B734" t="s">
+        <v>9</v>
+      </c>
+      <c r="C734" t="s">
+        <v>2</v>
+      </c>
+      <c r="D734" s="3">
+        <v>11841</v>
+      </c>
+      <c r="E734" s="3">
+        <v>1638</v>
+      </c>
+      <c r="F734">
+        <v>4.5</v>
+      </c>
+      <c r="G734">
+        <v>94</v>
+      </c>
+      <c r="H734">
+        <v>4.3</v>
+      </c>
+      <c r="I734">
+        <v>22</v>
+      </c>
+      <c r="J734">
+        <v>0.3</v>
+      </c>
+      <c r="K734">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="735" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A735" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B735" t="s">
+        <v>9</v>
+      </c>
+      <c r="C735" t="s">
+        <v>3</v>
+      </c>
+      <c r="D735" s="3">
+        <v>17230</v>
+      </c>
+      <c r="E735" s="3">
+        <v>3324</v>
+      </c>
+      <c r="F735">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G735">
+        <v>215</v>
+      </c>
+      <c r="H735">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I735">
+        <v>62</v>
+      </c>
+      <c r="J735">
+        <v>0.9</v>
+      </c>
+      <c r="K735">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A736" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B736" t="s">
+        <v>9</v>
+      </c>
+      <c r="C736" t="s">
+        <v>4</v>
+      </c>
+      <c r="D736" s="3">
+        <v>20412</v>
+      </c>
+      <c r="E736" s="3">
+        <v>5282</v>
+      </c>
+      <c r="F736">
+        <v>14.6</v>
+      </c>
+      <c r="G736">
+        <v>416</v>
+      </c>
+      <c r="H736">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I736">
+        <v>146</v>
+      </c>
+      <c r="J736">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K736">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="737" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A737" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B737" t="s">
+        <v>9</v>
+      </c>
+      <c r="C737" t="s">
+        <v>5</v>
+      </c>
+      <c r="D737" s="3">
+        <v>14303</v>
+      </c>
+      <c r="E737" s="3">
+        <v>6392</v>
+      </c>
+      <c r="F737">
+        <v>17.7</v>
+      </c>
+      <c r="G737">
+        <v>646</v>
+      </c>
+      <c r="H737">
+        <v>29.3</v>
+      </c>
+      <c r="I737">
+        <v>409</v>
+      </c>
+      <c r="J737">
+        <v>6.2</v>
+      </c>
+      <c r="K737">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="738" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A738" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B738" t="s">
+        <v>9</v>
+      </c>
+      <c r="C738" t="s">
+        <v>6</v>
+      </c>
+      <c r="D738" s="3">
+        <v>12974</v>
+      </c>
+      <c r="E738" s="3">
+        <v>7781</v>
+      </c>
+      <c r="F738">
+        <v>21.5</v>
+      </c>
+      <c r="G738">
+        <v>625</v>
+      </c>
+      <c r="H738">
+        <v>28.3</v>
+      </c>
+      <c r="I738" s="3">
+        <v>1259</v>
+      </c>
+      <c r="J738">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="K738">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="739" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A739" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B739" t="s">
+        <v>9</v>
+      </c>
+      <c r="C739" t="s">
+        <v>12</v>
+      </c>
+      <c r="D739" s="3">
+        <v>18264</v>
+      </c>
+      <c r="E739" s="3">
+        <v>7794</v>
+      </c>
+      <c r="F739">
+        <v>21.5</v>
+      </c>
+      <c r="G739">
+        <v>130</v>
+      </c>
+      <c r="H739">
+        <v>5.9</v>
+      </c>
+      <c r="I739" s="3">
+        <v>2852</v>
+      </c>
+      <c r="J739">
+        <v>43.3</v>
+      </c>
+      <c r="K739">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="740" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A740" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B740" t="s">
+        <v>9</v>
+      </c>
+      <c r="C740" t="s">
+        <v>13</v>
+      </c>
+      <c r="D740" s="3">
+        <v>10499</v>
+      </c>
+      <c r="E740" s="3">
+        <v>3060</v>
+      </c>
+      <c r="F740">
+        <v>8.5</v>
+      </c>
+      <c r="G740">
+        <v>22</v>
+      </c>
+      <c r="H740">
+        <v>1</v>
+      </c>
+      <c r="I740" s="3">
+        <v>1830</v>
+      </c>
+      <c r="J740">
+        <v>27.8</v>
+      </c>
+      <c r="K740">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="741" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A741" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B741" t="s">
+        <v>10</v>
+      </c>
+      <c r="C741" t="s">
+        <v>0</v>
+      </c>
+      <c r="D741">
+        <v>356</v>
+      </c>
+      <c r="E741">
+        <v>130</v>
+      </c>
+      <c r="F741">
+        <v>0.3</v>
+      </c>
+      <c r="G741">
+        <v>21</v>
+      </c>
+      <c r="H741">
+        <v>0.4</v>
+      </c>
+      <c r="I741">
+        <v>1</v>
+      </c>
+      <c r="J741">
+        <v>0</v>
+      </c>
+      <c r="K741">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="742" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A742" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B742" t="s">
+        <v>10</v>
+      </c>
+      <c r="C742" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D742">
+        <v>538</v>
+      </c>
+      <c r="E742">
+        <v>114</v>
+      </c>
+      <c r="F742">
+        <v>0.2</v>
+      </c>
+      <c r="G742">
+        <v>9</v>
+      </c>
+      <c r="H742">
+        <v>0.2</v>
+      </c>
+      <c r="I742">
+        <v>1</v>
+      </c>
+      <c r="J742">
+        <v>0</v>
+      </c>
+      <c r="K742">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="743" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A743" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B743" t="s">
+        <v>10</v>
+      </c>
+      <c r="C743" t="s">
+        <v>1</v>
+      </c>
+      <c r="D743" s="3">
+        <v>3701</v>
+      </c>
+      <c r="E743">
+        <v>628</v>
+      </c>
+      <c r="F743">
+        <v>1.3</v>
+      </c>
+      <c r="G743">
+        <v>45</v>
+      </c>
+      <c r="H743">
+        <v>0.9</v>
+      </c>
+      <c r="I743">
+        <v>14</v>
+      </c>
+      <c r="J743">
+        <v>0.2</v>
+      </c>
+      <c r="K743">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="744" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A744" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B744" t="s">
+        <v>10</v>
+      </c>
+      <c r="C744" t="s">
+        <v>2</v>
+      </c>
+      <c r="D744" s="3">
+        <v>7083</v>
+      </c>
+      <c r="E744" s="3">
+        <v>1791</v>
+      </c>
+      <c r="F744">
+        <v>3.8</v>
+      </c>
+      <c r="G744">
+        <v>156</v>
+      </c>
+      <c r="H744">
+        <v>3.1</v>
+      </c>
+      <c r="I744">
+        <v>33</v>
+      </c>
+      <c r="J744">
+        <v>0.4</v>
+      </c>
+      <c r="K744">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="745" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A745" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B745" t="s">
+        <v>10</v>
+      </c>
+      <c r="C745" t="s">
+        <v>3</v>
+      </c>
+      <c r="D745" s="3">
+        <v>12398</v>
+      </c>
+      <c r="E745" s="3">
+        <v>4724</v>
+      </c>
+      <c r="F745">
+        <v>9.9</v>
+      </c>
+      <c r="G745">
+        <v>480</v>
+      </c>
+      <c r="H745">
+        <v>9.5</v>
+      </c>
+      <c r="I745">
+        <v>110</v>
+      </c>
+      <c r="J745">
+        <v>1.2</v>
+      </c>
+      <c r="K745">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="746" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A746" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B746" t="s">
+        <v>10</v>
+      </c>
+      <c r="C746" t="s">
+        <v>4</v>
+      </c>
+      <c r="D746" s="3">
+        <v>16009</v>
+      </c>
+      <c r="E746" s="3">
+        <v>7765</v>
+      </c>
+      <c r="F746">
+        <v>16.3</v>
+      </c>
+      <c r="G746" s="3">
+        <v>1020</v>
+      </c>
+      <c r="H746">
+        <v>20.3</v>
+      </c>
+      <c r="I746">
+        <v>351</v>
+      </c>
+      <c r="J746">
+        <v>3.8</v>
+      </c>
+      <c r="K746">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="747" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A747" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B747" t="s">
+        <v>10</v>
+      </c>
+      <c r="C747" t="s">
+        <v>5</v>
+      </c>
+      <c r="D747" s="3">
+        <v>16054</v>
+      </c>
+      <c r="E747" s="3">
+        <v>9846</v>
+      </c>
+      <c r="F747">
+        <v>20.7</v>
+      </c>
+      <c r="G747" s="3">
+        <v>1673</v>
+      </c>
+      <c r="H747">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I747">
+        <v>978</v>
+      </c>
+      <c r="J747">
+        <v>10.6</v>
+      </c>
+      <c r="K747">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="748" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A748" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B748" t="s">
+        <v>10</v>
+      </c>
+      <c r="C748" t="s">
+        <v>6</v>
+      </c>
+      <c r="D748" s="3">
+        <v>16575</v>
+      </c>
+      <c r="E748" s="3">
+        <v>11669</v>
+      </c>
+      <c r="F748">
+        <v>24.6</v>
+      </c>
+      <c r="G748" s="3">
+        <v>1444</v>
+      </c>
+      <c r="H748">
+        <v>28.7</v>
+      </c>
+      <c r="I748" s="3">
+        <v>2753</v>
+      </c>
+      <c r="J748">
+        <v>29.7</v>
+      </c>
+      <c r="K748">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="749" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A749" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B749" t="s">
+        <v>10</v>
+      </c>
+      <c r="C749" t="s">
+        <v>12</v>
+      </c>
+      <c r="D749" s="3">
+        <v>13932</v>
+      </c>
+      <c r="E749" s="3">
+        <v>8806</v>
+      </c>
+      <c r="F749">
+        <v>18.5</v>
+      </c>
+      <c r="G749">
+        <v>163</v>
+      </c>
+      <c r="H749">
+        <v>3.2</v>
+      </c>
+      <c r="I749" s="3">
+        <v>3769</v>
+      </c>
+      <c r="J749">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="K749">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="750" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A750" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B750" t="s">
+        <v>10</v>
+      </c>
+      <c r="C750" t="s">
+        <v>13</v>
+      </c>
+      <c r="D750" s="3">
+        <v>4278</v>
+      </c>
+      <c r="E750" s="3">
+        <v>2052</v>
+      </c>
+      <c r="F750">
+        <v>4.3</v>
+      </c>
+      <c r="G750">
+        <v>16</v>
+      </c>
+      <c r="H750">
+        <v>0.3</v>
+      </c>
+      <c r="I750" s="3">
+        <v>1251</v>
+      </c>
+      <c r="J750">
+        <v>13.5</v>
+      </c>
+      <c r="K750">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="751" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A751" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B751" t="s">
+        <v>9</v>
+      </c>
+      <c r="C751" t="s">
+        <v>0</v>
+      </c>
+      <c r="D751">
+        <v>307</v>
+      </c>
+      <c r="E751">
+        <v>101</v>
+      </c>
+      <c r="F751">
+        <v>0.3</v>
+      </c>
+      <c r="G751">
+        <v>11</v>
+      </c>
+      <c r="H751">
+        <v>0.5</v>
+      </c>
+      <c r="I751">
+        <v>1</v>
+      </c>
+      <c r="J751">
+        <v>0</v>
+      </c>
+      <c r="K751">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="752" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A752" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B752" t="s">
+        <v>9</v>
+      </c>
+      <c r="C752" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D752">
+        <v>675</v>
+      </c>
+      <c r="E752">
+        <v>124</v>
+      </c>
+      <c r="F752">
+        <v>0.3</v>
+      </c>
+      <c r="G752">
+        <v>8</v>
+      </c>
+      <c r="H752">
+        <v>0.4</v>
+      </c>
+      <c r="I752">
+        <v>3</v>
+      </c>
+      <c r="J752">
+        <v>0</v>
+      </c>
+      <c r="K752">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="753" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A753" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B753" t="s">
+        <v>9</v>
+      </c>
+      <c r="C753" t="s">
+        <v>1</v>
+      </c>
+      <c r="D753" s="3">
+        <v>7455</v>
+      </c>
+      <c r="E753">
+        <v>699</v>
+      </c>
+      <c r="F753">
+        <v>1.9</v>
+      </c>
+      <c r="G753">
+        <v>38</v>
+      </c>
+      <c r="H753">
+        <v>1.7</v>
+      </c>
+      <c r="I753">
+        <v>8</v>
+      </c>
+      <c r="J753">
+        <v>0.1</v>
+      </c>
+      <c r="K753">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="754" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A754" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B754" t="s">
+        <v>9</v>
+      </c>
+      <c r="C754" t="s">
+        <v>2</v>
+      </c>
+      <c r="D754" s="3">
+        <v>11870</v>
+      </c>
+      <c r="E754" s="3">
+        <v>1644</v>
+      </c>
+      <c r="F754">
+        <v>4.5</v>
+      </c>
+      <c r="G754">
+        <v>94</v>
+      </c>
+      <c r="H754">
+        <v>4.3</v>
+      </c>
+      <c r="I754">
+        <v>22</v>
+      </c>
+      <c r="J754">
+        <v>0.3</v>
+      </c>
+      <c r="K754">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="755" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A755" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B755" t="s">
+        <v>9</v>
+      </c>
+      <c r="C755" t="s">
+        <v>3</v>
+      </c>
+      <c r="D755" s="3">
+        <v>17264</v>
+      </c>
+      <c r="E755" s="3">
+        <v>3344</v>
+      </c>
+      <c r="F755">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G755">
+        <v>215</v>
+      </c>
+      <c r="H755">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I755">
+        <v>62</v>
+      </c>
+      <c r="J755">
+        <v>0.9</v>
+      </c>
+      <c r="K755">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="756" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A756" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B756" t="s">
+        <v>9</v>
+      </c>
+      <c r="C756" t="s">
+        <v>4</v>
+      </c>
+      <c r="D756" s="3">
+        <v>20444</v>
+      </c>
+      <c r="E756" s="3">
+        <v>5294</v>
+      </c>
+      <c r="F756">
+        <v>14.6</v>
+      </c>
+      <c r="G756">
+        <v>417</v>
+      </c>
+      <c r="H756">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I756">
+        <v>146</v>
+      </c>
+      <c r="J756">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K756">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="757" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A757" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B757" t="s">
+        <v>9</v>
+      </c>
+      <c r="C757" t="s">
+        <v>5</v>
+      </c>
+      <c r="D757" s="3">
+        <v>14325</v>
+      </c>
+      <c r="E757" s="3">
+        <v>6405</v>
+      </c>
+      <c r="F757">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G757">
+        <v>648</v>
+      </c>
+      <c r="H757">
+        <v>29.3</v>
+      </c>
+      <c r="I757">
+        <v>411</v>
+      </c>
+      <c r="J757">
+        <v>6.2</v>
+      </c>
+      <c r="K757">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="758" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A758" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B758" t="s">
+        <v>9</v>
+      </c>
+      <c r="C758" t="s">
+        <v>6</v>
+      </c>
+      <c r="D758" s="3">
+        <v>12983</v>
+      </c>
+      <c r="E758" s="3">
+        <v>7797</v>
+      </c>
+      <c r="F758">
+        <v>21.5</v>
+      </c>
+      <c r="G758">
+        <v>626</v>
+      </c>
+      <c r="H758">
+        <v>28.3</v>
+      </c>
+      <c r="I758" s="3">
+        <v>1264</v>
+      </c>
+      <c r="J758">
+        <v>19</v>
+      </c>
+      <c r="K758">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="759" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A759" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B759" t="s">
+        <v>9</v>
+      </c>
+      <c r="C759" t="s">
+        <v>12</v>
+      </c>
+      <c r="D759" s="3">
+        <v>18238</v>
+      </c>
+      <c r="E759" s="3">
+        <v>7817</v>
+      </c>
+      <c r="F759">
+        <v>21.5</v>
+      </c>
+      <c r="G759">
+        <v>132</v>
+      </c>
+      <c r="H759">
+        <v>6</v>
+      </c>
+      <c r="I759" s="3">
+        <v>2878</v>
+      </c>
+      <c r="J759">
+        <v>43.2</v>
+      </c>
+      <c r="K759">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="760" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A760" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B760" t="s">
+        <v>9</v>
+      </c>
+      <c r="C760" t="s">
+        <v>13</v>
+      </c>
+      <c r="D760" s="3">
+        <v>10487</v>
+      </c>
+      <c r="E760" s="3">
+        <v>3072</v>
+      </c>
+      <c r="F760">
+        <v>8.5</v>
+      </c>
+      <c r="G760">
+        <v>22</v>
+      </c>
+      <c r="H760">
+        <v>1</v>
+      </c>
+      <c r="I760" s="3">
+        <v>1861</v>
+      </c>
+      <c r="J760">
+        <v>28</v>
+      </c>
+      <c r="K760">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="761" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A761" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B761" t="s">
+        <v>10</v>
+      </c>
+      <c r="C761" t="s">
+        <v>0</v>
+      </c>
+      <c r="D761">
+        <v>363</v>
+      </c>
+      <c r="E761">
+        <v>130</v>
+      </c>
+      <c r="F761">
+        <v>0.3</v>
+      </c>
+      <c r="G761">
+        <v>21</v>
+      </c>
+      <c r="H761">
+        <v>0.4</v>
+      </c>
+      <c r="I761">
+        <v>1</v>
+      </c>
+      <c r="J761">
+        <v>0</v>
+      </c>
+      <c r="K761">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="762" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A762" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B762" t="s">
+        <v>10</v>
+      </c>
+      <c r="C762" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D762">
+        <v>544</v>
+      </c>
+      <c r="E762">
+        <v>115</v>
+      </c>
+      <c r="F762">
+        <v>0.2</v>
+      </c>
+      <c r="G762">
+        <v>9</v>
+      </c>
+      <c r="H762">
+        <v>0.2</v>
+      </c>
+      <c r="I762">
+        <v>1</v>
+      </c>
+      <c r="J762">
+        <v>0</v>
+      </c>
+      <c r="K762">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="763" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A763" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B763" t="s">
+        <v>10</v>
+      </c>
+      <c r="C763" t="s">
+        <v>1</v>
+      </c>
+      <c r="D763" s="3">
+        <v>3707</v>
+      </c>
+      <c r="E763">
+        <v>633</v>
+      </c>
+      <c r="F763">
+        <v>1.3</v>
+      </c>
+      <c r="G763">
+        <v>46</v>
+      </c>
+      <c r="H763">
+        <v>0.9</v>
+      </c>
+      <c r="I763">
+        <v>14</v>
+      </c>
+      <c r="J763">
+        <v>0.2</v>
+      </c>
+      <c r="K763">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="764" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A764" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B764" t="s">
+        <v>10</v>
+      </c>
+      <c r="C764" t="s">
+        <v>2</v>
+      </c>
+      <c r="D764" s="3">
+        <v>7105</v>
+      </c>
+      <c r="E764" s="3">
+        <v>1794</v>
+      </c>
+      <c r="F764">
+        <v>3.8</v>
+      </c>
+      <c r="G764">
+        <v>156</v>
+      </c>
+      <c r="H764">
+        <v>3.1</v>
+      </c>
+      <c r="I764">
+        <v>33</v>
+      </c>
+      <c r="J764">
+        <v>0.4</v>
+      </c>
+      <c r="K764">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="765" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A765" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B765" t="s">
+        <v>10</v>
+      </c>
+      <c r="C765" t="s">
+        <v>3</v>
+      </c>
+      <c r="D765" s="3">
+        <v>12415</v>
+      </c>
+      <c r="E765" s="3">
+        <v>4737</v>
+      </c>
+      <c r="F765">
+        <v>9.9</v>
+      </c>
+      <c r="G765">
+        <v>480</v>
+      </c>
+      <c r="H765">
+        <v>9.5</v>
+      </c>
+      <c r="I765">
+        <v>110</v>
+      </c>
+      <c r="J765">
+        <v>1.2</v>
+      </c>
+      <c r="K765">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="766" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A766" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B766" t="s">
+        <v>10</v>
+      </c>
+      <c r="C766" t="s">
+        <v>4</v>
+      </c>
+      <c r="D766" s="3">
+        <v>16035</v>
+      </c>
+      <c r="E766" s="3">
+        <v>7782</v>
+      </c>
+      <c r="F766">
+        <v>16.3</v>
+      </c>
+      <c r="G766" s="3">
+        <v>1021</v>
+      </c>
+      <c r="H766">
+        <v>20.3</v>
+      </c>
+      <c r="I766">
+        <v>353</v>
+      </c>
+      <c r="J766">
+        <v>3.8</v>
+      </c>
+      <c r="K766">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="767" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A767" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B767" t="s">
+        <v>10</v>
+      </c>
+      <c r="C767" t="s">
+        <v>5</v>
+      </c>
+      <c r="D767" s="3">
+        <v>16065</v>
+      </c>
+      <c r="E767" s="3">
+        <v>9860</v>
+      </c>
+      <c r="F767">
+        <v>20.7</v>
+      </c>
+      <c r="G767" s="3">
+        <v>1677</v>
+      </c>
+      <c r="H767">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I767">
+        <v>982</v>
+      </c>
+      <c r="J767">
+        <v>10.6</v>
+      </c>
+      <c r="K767">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="768" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A768" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B768" t="s">
+        <v>10</v>
+      </c>
+      <c r="C768" t="s">
+        <v>6</v>
+      </c>
+      <c r="D768" s="3">
+        <v>16580</v>
+      </c>
+      <c r="E768" s="3">
+        <v>11688</v>
+      </c>
+      <c r="F768">
+        <v>24.5</v>
+      </c>
+      <c r="G768" s="3">
+        <v>1448</v>
+      </c>
+      <c r="H768">
+        <v>28.7</v>
+      </c>
+      <c r="I768" s="3">
+        <v>2760</v>
+      </c>
+      <c r="J768">
+        <v>29.7</v>
+      </c>
+      <c r="K768">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="769" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A769" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B769" t="s">
+        <v>10</v>
+      </c>
+      <c r="C769" t="s">
+        <v>12</v>
+      </c>
+      <c r="D769" s="3">
+        <v>13933</v>
+      </c>
+      <c r="E769" s="3">
+        <v>8828</v>
+      </c>
+      <c r="F769">
+        <v>18.5</v>
+      </c>
+      <c r="G769">
+        <v>164</v>
+      </c>
+      <c r="H769">
+        <v>3.3</v>
+      </c>
+      <c r="I769" s="3">
+        <v>3783</v>
+      </c>
+      <c r="J769">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="K769">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="770" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A770" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B770" t="s">
+        <v>10</v>
+      </c>
+      <c r="C770" t="s">
+        <v>13</v>
+      </c>
+      <c r="D770" s="3">
+        <v>4282</v>
+      </c>
+      <c r="E770" s="3">
+        <v>2061</v>
+      </c>
+      <c r="F770">
+        <v>4.3</v>
+      </c>
+      <c r="G770">
+        <v>16</v>
+      </c>
+      <c r="H770">
+        <v>0.3</v>
+      </c>
+      <c r="I770" s="3">
+        <v>1263</v>
+      </c>
+      <c r="J770">
+        <v>13.6</v>
+      </c>
+      <c r="K770">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="771" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A771" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B771" t="s">
+        <v>9</v>
+      </c>
+      <c r="C771" t="s">
+        <v>0</v>
+      </c>
+      <c r="D771">
+        <v>317</v>
+      </c>
+      <c r="E771">
+        <v>102</v>
+      </c>
+      <c r="F771">
+        <v>0.3</v>
+      </c>
+      <c r="G771">
+        <v>11</v>
+      </c>
+      <c r="H771">
+        <v>0.5</v>
+      </c>
+      <c r="I771">
+        <v>1</v>
+      </c>
+      <c r="J771">
+        <v>0</v>
+      </c>
+      <c r="K771">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="772" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A772" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B772" t="s">
+        <v>9</v>
+      </c>
+      <c r="C772" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D772">
+        <v>696</v>
+      </c>
+      <c r="E772">
+        <v>123</v>
+      </c>
+      <c r="F772">
+        <v>0.3</v>
+      </c>
+      <c r="G772">
+        <v>8</v>
+      </c>
+      <c r="H772">
+        <v>0.4</v>
+      </c>
+      <c r="I772">
+        <v>3</v>
+      </c>
+      <c r="J772">
+        <v>0</v>
+      </c>
+      <c r="K772">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="773" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A773" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B773" t="s">
+        <v>9</v>
+      </c>
+      <c r="C773" t="s">
+        <v>1</v>
+      </c>
+      <c r="D773" s="3">
+        <v>7725</v>
+      </c>
+      <c r="E773">
+        <v>705</v>
+      </c>
+      <c r="F773">
+        <v>1.9</v>
+      </c>
+      <c r="G773">
+        <v>37</v>
+      </c>
+      <c r="H773">
+        <v>1.6</v>
+      </c>
+      <c r="I773">
+        <v>8</v>
+      </c>
+      <c r="J773">
+        <v>0.1</v>
+      </c>
+      <c r="K773">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="774" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A774" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B774" t="s">
+        <v>9</v>
+      </c>
+      <c r="C774" t="s">
+        <v>2</v>
+      </c>
+      <c r="D774" s="3">
+        <v>12280</v>
+      </c>
+      <c r="E774" s="3">
+        <v>1667</v>
+      </c>
+      <c r="F774">
+        <v>4.5</v>
+      </c>
+      <c r="G774">
+        <v>92</v>
+      </c>
+      <c r="H774">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I774">
+        <v>21</v>
+      </c>
+      <c r="J774">
+        <v>0.3</v>
+      </c>
+      <c r="K774">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="775" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A775" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B775" t="s">
+        <v>9</v>
+      </c>
+      <c r="C775" t="s">
+        <v>3</v>
+      </c>
+      <c r="D775" s="3">
+        <v>17890</v>
+      </c>
+      <c r="E775" s="3">
+        <v>3373</v>
+      </c>
+      <c r="F775">
+        <v>9.1</v>
+      </c>
+      <c r="G775">
+        <v>218</v>
+      </c>
+      <c r="H775">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I775">
+        <v>64</v>
+      </c>
+      <c r="J775">
+        <v>0.9</v>
+      </c>
+      <c r="K775">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="776" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A776" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B776" t="s">
+        <v>9</v>
+      </c>
+      <c r="C776" t="s">
+        <v>4</v>
+      </c>
+      <c r="D776" s="3">
+        <v>21167</v>
+      </c>
+      <c r="E776" s="3">
+        <v>5356</v>
+      </c>
+      <c r="F776">
+        <v>14.5</v>
+      </c>
+      <c r="G776">
+        <v>422</v>
+      </c>
+      <c r="H776">
+        <v>18.7</v>
+      </c>
+      <c r="I776">
+        <v>149</v>
+      </c>
+      <c r="J776">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K776">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="777" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A777" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B777" t="s">
+        <v>9</v>
+      </c>
+      <c r="C777" t="s">
+        <v>5</v>
+      </c>
+      <c r="D777" s="3">
+        <v>14627</v>
+      </c>
+      <c r="E777" s="3">
+        <v>6454</v>
+      </c>
+      <c r="F777">
+        <v>17.5</v>
+      </c>
+      <c r="G777">
+        <v>659</v>
+      </c>
+      <c r="H777">
+        <v>29.2</v>
+      </c>
+      <c r="I777">
+        <v>423</v>
+      </c>
+      <c r="J777">
+        <v>6.1</v>
+      </c>
+      <c r="K777">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="778" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A778" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B778" t="s">
+        <v>9</v>
+      </c>
+      <c r="C778" t="s">
+        <v>6</v>
+      </c>
+      <c r="D778" s="3">
+        <v>13228</v>
+      </c>
+      <c r="E778" s="3">
+        <v>7889</v>
+      </c>
+      <c r="F778">
+        <v>21.4</v>
+      </c>
+      <c r="G778">
+        <v>642</v>
+      </c>
+      <c r="H778">
+        <v>28.5</v>
+      </c>
+      <c r="I778" s="3">
+        <v>1298</v>
+      </c>
+      <c r="J778">
+        <v>18.7</v>
+      </c>
+      <c r="K778">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="779" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A779" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B779" t="s">
+        <v>9</v>
+      </c>
+      <c r="C779" t="s">
+        <v>12</v>
+      </c>
+      <c r="D779" s="3">
+        <v>18832</v>
+      </c>
+      <c r="E779" s="3">
+        <v>8011</v>
+      </c>
+      <c r="F779">
+        <v>21.7</v>
+      </c>
+      <c r="G779">
+        <v>139</v>
+      </c>
+      <c r="H779">
+        <v>6.2</v>
+      </c>
+      <c r="I779" s="3">
+        <v>2991</v>
+      </c>
+      <c r="J779">
+        <v>43.2</v>
+      </c>
+      <c r="K779">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="780" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A780" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B780" t="s">
+        <v>9</v>
+      </c>
+      <c r="C780" t="s">
+        <v>13</v>
+      </c>
+      <c r="D780" s="3">
+        <v>10889</v>
+      </c>
+      <c r="E780" s="3">
+        <v>3202</v>
+      </c>
+      <c r="F780">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G780">
+        <v>25</v>
+      </c>
+      <c r="H780">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I780" s="3">
+        <v>1971</v>
+      </c>
+      <c r="J780">
+        <v>28.4</v>
+      </c>
+      <c r="K780">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="781" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A781" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B781" t="s">
+        <v>10</v>
+      </c>
+      <c r="C781" t="s">
+        <v>0</v>
+      </c>
+      <c r="D781">
+        <v>377</v>
+      </c>
+      <c r="E781">
+        <v>132</v>
+      </c>
+      <c r="F781">
+        <v>0.3</v>
+      </c>
+      <c r="G781">
+        <v>21</v>
+      </c>
+      <c r="H781">
+        <v>0.4</v>
+      </c>
+      <c r="I781">
+        <v>1</v>
+      </c>
+      <c r="J781">
+        <v>0</v>
+      </c>
+      <c r="K781">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="782" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A782" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B782" t="s">
+        <v>10</v>
+      </c>
+      <c r="C782" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D782">
+        <v>562</v>
+      </c>
+      <c r="E782">
+        <v>116</v>
+      </c>
+      <c r="F782">
+        <v>0.2</v>
+      </c>
+      <c r="G782">
+        <v>10</v>
+      </c>
+      <c r="H782">
+        <v>0.2</v>
+      </c>
+      <c r="I782">
+        <v>2</v>
+      </c>
+      <c r="J782">
+        <v>0</v>
+      </c>
+      <c r="K782">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="783" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A783" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B783" t="s">
+        <v>10</v>
+      </c>
+      <c r="C783" t="s">
+        <v>1</v>
+      </c>
+      <c r="D783" s="3">
+        <v>3815</v>
+      </c>
+      <c r="E783">
+        <v>643</v>
+      </c>
+      <c r="F783">
+        <v>1.3</v>
+      </c>
+      <c r="G783">
+        <v>49</v>
+      </c>
+      <c r="H783">
+        <v>1</v>
+      </c>
+      <c r="I783">
+        <v>14</v>
+      </c>
+      <c r="J783">
+        <v>0.1</v>
+      </c>
+      <c r="K783">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="784" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A784" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B784" t="s">
+        <v>10</v>
+      </c>
+      <c r="C784" t="s">
+        <v>2</v>
+      </c>
+      <c r="D784" s="3">
+        <v>7278</v>
+      </c>
+      <c r="E784" s="3">
+        <v>1799</v>
+      </c>
+      <c r="F784">
+        <v>3.7</v>
+      </c>
+      <c r="G784">
+        <v>157</v>
+      </c>
+      <c r="H784">
+        <v>3.1</v>
+      </c>
+      <c r="I784">
+        <v>34</v>
+      </c>
+      <c r="J784">
+        <v>0.4</v>
+      </c>
+      <c r="K784">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="785" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A785" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B785" t="s">
+        <v>10</v>
+      </c>
+      <c r="C785" t="s">
+        <v>3</v>
+      </c>
+      <c r="D785" s="3">
+        <v>12682</v>
+      </c>
+      <c r="E785" s="3">
+        <v>4754</v>
+      </c>
+      <c r="F785">
+        <v>9.9</v>
+      </c>
+      <c r="G785">
+        <v>483</v>
+      </c>
+      <c r="H785">
+        <v>9.5</v>
+      </c>
+      <c r="I785">
+        <v>110</v>
+      </c>
+      <c r="J785">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K785">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="786" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A786" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B786" t="s">
+        <v>10</v>
+      </c>
+      <c r="C786" t="s">
+        <v>4</v>
+      </c>
+      <c r="D786" s="3">
+        <v>16387</v>
+      </c>
+      <c r="E786" s="3">
+        <v>7852</v>
+      </c>
+      <c r="F786">
+        <v>16.3</v>
+      </c>
+      <c r="G786" s="3">
+        <v>1028</v>
+      </c>
+      <c r="H786">
+        <v>20.2</v>
+      </c>
+      <c r="I786">
+        <v>374</v>
+      </c>
+      <c r="J786">
+        <v>3.9</v>
+      </c>
+      <c r="K786">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="787" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A787" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B787" t="s">
+        <v>10</v>
+      </c>
+      <c r="C787" t="s">
+        <v>5</v>
+      </c>
+      <c r="D787" s="3">
+        <v>16300</v>
+      </c>
+      <c r="E787" s="3">
+        <v>9924</v>
+      </c>
+      <c r="F787">
+        <v>20.6</v>
+      </c>
+      <c r="G787" s="3">
+        <v>1690</v>
+      </c>
+      <c r="H787">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="I787" s="3">
+        <v>1022</v>
+      </c>
+      <c r="J787">
+        <v>10.7</v>
+      </c>
+      <c r="K787">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="788" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A788" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B788" t="s">
+        <v>10</v>
+      </c>
+      <c r="C788" t="s">
+        <v>6</v>
+      </c>
+      <c r="D788" s="3">
+        <v>16750</v>
+      </c>
+      <c r="E788" s="3">
+        <v>11800</v>
+      </c>
+      <c r="F788">
+        <v>24.5</v>
+      </c>
+      <c r="G788" s="3">
+        <v>1464</v>
+      </c>
+      <c r="H788">
+        <v>28.8</v>
+      </c>
+      <c r="I788" s="3">
+        <v>2821</v>
+      </c>
+      <c r="J788">
+        <v>29.4</v>
+      </c>
+      <c r="K788">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="789" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A789" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B789" t="s">
+        <v>10</v>
+      </c>
+      <c r="C789" t="s">
+        <v>12</v>
+      </c>
+      <c r="D789" s="3">
+        <v>14207</v>
+      </c>
+      <c r="E789" s="3">
+        <v>8984</v>
+      </c>
+      <c r="F789">
+        <v>18.7</v>
+      </c>
+      <c r="G789">
+        <v>171</v>
+      </c>
+      <c r="H789">
+        <v>3.4</v>
+      </c>
+      <c r="I789" s="3">
+        <v>3885</v>
+      </c>
+      <c r="J789">
+        <v>40.5</v>
+      </c>
+      <c r="K789">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="790" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A790" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B790" t="s">
+        <v>10</v>
+      </c>
+      <c r="C790" t="s">
+        <v>13</v>
+      </c>
+      <c r="D790" s="3">
+        <v>4390</v>
+      </c>
+      <c r="E790" s="3">
+        <v>2123</v>
+      </c>
+      <c r="F790">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G790">
+        <v>18</v>
+      </c>
+      <c r="H790">
+        <v>0.4</v>
+      </c>
+      <c r="I790" s="3">
+        <v>1325</v>
+      </c>
+      <c r="J790">
+        <v>13.8</v>
+      </c>
+      <c r="K790">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="791" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A791" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B791" t="s">
+        <v>9</v>
+      </c>
+      <c r="C791" t="s">
+        <v>0</v>
+      </c>
+      <c r="D791">
+        <v>317</v>
+      </c>
+      <c r="E791">
+        <v>102</v>
+      </c>
+      <c r="F791">
+        <v>0.3</v>
+      </c>
+      <c r="G791">
+        <v>11</v>
+      </c>
+      <c r="H791">
+        <v>0.5</v>
+      </c>
+      <c r="I791">
+        <v>1</v>
+      </c>
+      <c r="J791">
+        <v>0</v>
+      </c>
+      <c r="K791">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="792" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A792" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B792" t="s">
+        <v>9</v>
+      </c>
+      <c r="C792" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D792">
+        <v>700</v>
+      </c>
+      <c r="E792">
+        <v>123</v>
+      </c>
+      <c r="F792">
+        <v>0.3</v>
+      </c>
+      <c r="G792">
+        <v>8</v>
+      </c>
+      <c r="H792">
+        <v>0.4</v>
+      </c>
+      <c r="I792">
+        <v>3</v>
+      </c>
+      <c r="J792">
+        <v>0</v>
+      </c>
+      <c r="K792">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="793" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A793" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B793" t="s">
+        <v>9</v>
+      </c>
+      <c r="C793" t="s">
+        <v>1</v>
+      </c>
+      <c r="D793" s="3">
+        <v>7760</v>
+      </c>
+      <c r="E793">
+        <v>707</v>
+      </c>
+      <c r="F793">
+        <v>1.9</v>
+      </c>
+      <c r="G793">
+        <v>37</v>
+      </c>
+      <c r="H793">
+        <v>1.6</v>
+      </c>
+      <c r="I793">
+        <v>8</v>
+      </c>
+      <c r="J793">
+        <v>0.1</v>
+      </c>
+      <c r="K793">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="794" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A794" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B794" t="s">
+        <v>9</v>
+      </c>
+      <c r="C794" t="s">
+        <v>2</v>
+      </c>
+      <c r="D794" s="3">
+        <v>12352</v>
+      </c>
+      <c r="E794" s="3">
+        <v>1670</v>
+      </c>
+      <c r="F794">
+        <v>4.5</v>
+      </c>
+      <c r="G794">
+        <v>93</v>
+      </c>
+      <c r="H794">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I794">
+        <v>22</v>
+      </c>
+      <c r="J794">
+        <v>0.3</v>
+      </c>
+      <c r="K794">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="795" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A795" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B795" t="s">
+        <v>9</v>
+      </c>
+      <c r="C795" t="s">
+        <v>3</v>
+      </c>
+      <c r="D795" s="3">
+        <v>17984</v>
+      </c>
+      <c r="E795" s="3">
+        <v>3383</v>
+      </c>
+      <c r="F795">
+        <v>9.1</v>
+      </c>
+      <c r="G795">
+        <v>219</v>
+      </c>
+      <c r="H795">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I795">
+        <v>64</v>
+      </c>
+      <c r="J795">
+        <v>0.9</v>
+      </c>
+      <c r="K795">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="796" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A796" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B796" t="s">
+        <v>9</v>
+      </c>
+      <c r="C796" t="s">
+        <v>4</v>
+      </c>
+      <c r="D796" s="3">
+        <v>21305</v>
+      </c>
+      <c r="E796" s="3">
+        <v>5373</v>
+      </c>
+      <c r="F796">
+        <v>14.5</v>
+      </c>
+      <c r="G796">
+        <v>423</v>
+      </c>
+      <c r="H796">
+        <v>18.7</v>
+      </c>
+      <c r="I796">
+        <v>149</v>
+      </c>
+      <c r="J796">
+        <v>2.1</v>
+      </c>
+      <c r="K796">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="797" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A797" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B797" t="s">
+        <v>9</v>
+      </c>
+      <c r="C797" t="s">
+        <v>5</v>
+      </c>
+      <c r="D797" s="3">
+        <v>14717</v>
+      </c>
+      <c r="E797" s="3">
+        <v>6473</v>
+      </c>
+      <c r="F797">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G797">
+        <v>660</v>
+      </c>
+      <c r="H797">
+        <v>29.2</v>
+      </c>
+      <c r="I797">
+        <v>426</v>
+      </c>
+      <c r="J797">
+        <v>6.1</v>
+      </c>
+      <c r="K797">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="798" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A798" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B798" t="s">
+        <v>9</v>
+      </c>
+      <c r="C798" t="s">
+        <v>6</v>
+      </c>
+      <c r="D798" s="3">
+        <v>13299</v>
+      </c>
+      <c r="E798" s="3">
+        <v>7925</v>
+      </c>
+      <c r="F798">
+        <v>21.3</v>
+      </c>
+      <c r="G798">
+        <v>643</v>
+      </c>
+      <c r="H798">
+        <v>28.5</v>
+      </c>
+      <c r="I798" s="3">
+        <v>1308</v>
+      </c>
+      <c r="J798">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K798">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="799" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A799" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B799" t="s">
+        <v>9</v>
+      </c>
+      <c r="C799" t="s">
+        <v>12</v>
+      </c>
+      <c r="D799" s="3">
+        <v>18972</v>
+      </c>
+      <c r="E799" s="3">
+        <v>8113</v>
+      </c>
+      <c r="F799">
+        <v>21.8</v>
+      </c>
+      <c r="G799">
+        <v>140</v>
+      </c>
+      <c r="H799">
+        <v>6.2</v>
+      </c>
+      <c r="I799" s="3">
+        <v>3015</v>
+      </c>
+      <c r="J799">
+        <v>43</v>
+      </c>
+      <c r="K799">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="800" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A800" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B800" t="s">
+        <v>9</v>
+      </c>
+      <c r="C800" t="s">
+        <v>13</v>
+      </c>
+      <c r="D800" s="3">
+        <v>11028</v>
+      </c>
+      <c r="E800" s="3">
+        <v>3286</v>
+      </c>
+      <c r="F800">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G800">
+        <v>26</v>
+      </c>
+      <c r="H800">
+        <v>1.2</v>
+      </c>
+      <c r="I800" s="3">
+        <v>2018</v>
+      </c>
+      <c r="J800">
+        <v>28.8</v>
+      </c>
+      <c r="K800">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="801" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A801" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B801" t="s">
+        <v>10</v>
+      </c>
+      <c r="C801" t="s">
+        <v>0</v>
+      </c>
+      <c r="D801">
+        <v>379</v>
+      </c>
+      <c r="E801">
+        <v>132</v>
+      </c>
+      <c r="F801">
+        <v>0.3</v>
+      </c>
+      <c r="G801">
+        <v>21</v>
+      </c>
+      <c r="H801">
+        <v>0.4</v>
+      </c>
+      <c r="I801">
+        <v>1</v>
+      </c>
+      <c r="J801">
+        <v>0</v>
+      </c>
+      <c r="K801">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="802" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A802" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B802" t="s">
+        <v>10</v>
+      </c>
+      <c r="C802" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D802">
+        <v>569</v>
+      </c>
+      <c r="E802">
+        <v>116</v>
+      </c>
+      <c r="F802">
+        <v>0.2</v>
+      </c>
+      <c r="G802">
+        <v>10</v>
+      </c>
+      <c r="H802">
+        <v>0.2</v>
+      </c>
+      <c r="I802">
+        <v>2</v>
+      </c>
+      <c r="J802">
+        <v>0</v>
+      </c>
+      <c r="K802">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="803" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A803" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B803" t="s">
+        <v>10</v>
+      </c>
+      <c r="C803" t="s">
+        <v>1</v>
+      </c>
+      <c r="D803" s="3">
+        <v>3834</v>
+      </c>
+      <c r="E803">
+        <v>644</v>
+      </c>
+      <c r="F803">
+        <v>1.3</v>
+      </c>
+      <c r="G803">
+        <v>49</v>
+      </c>
+      <c r="H803">
+        <v>1</v>
+      </c>
+      <c r="I803">
+        <v>14</v>
+      </c>
+      <c r="J803">
+        <v>0.1</v>
+      </c>
+      <c r="K803">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="804" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A804" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B804" t="s">
+        <v>10</v>
+      </c>
+      <c r="C804" t="s">
+        <v>2</v>
+      </c>
+      <c r="D804" s="3">
+        <v>7306</v>
+      </c>
+      <c r="E804" s="3">
+        <v>1804</v>
+      </c>
+      <c r="F804">
+        <v>3.7</v>
+      </c>
+      <c r="G804">
+        <v>157</v>
+      </c>
+      <c r="H804">
+        <v>3.1</v>
+      </c>
+      <c r="I804">
+        <v>34</v>
+      </c>
+      <c r="J804">
+        <v>0.4</v>
+      </c>
+      <c r="K804">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="805" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A805" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B805" t="s">
+        <v>10</v>
+      </c>
+      <c r="C805" t="s">
+        <v>3</v>
+      </c>
+      <c r="D805" s="3">
+        <v>12722</v>
+      </c>
+      <c r="E805" s="3">
+        <v>4764</v>
+      </c>
+      <c r="F805">
+        <v>9.9</v>
+      </c>
+      <c r="G805">
+        <v>483</v>
+      </c>
+      <c r="H805">
+        <v>9.5</v>
+      </c>
+      <c r="I805">
+        <v>110</v>
+      </c>
+      <c r="J805">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K805">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="806" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A806" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B806" t="s">
+        <v>10</v>
+      </c>
+      <c r="C806" t="s">
+        <v>4</v>
+      </c>
+      <c r="D806" s="3">
+        <v>16463</v>
+      </c>
+      <c r="E806" s="3">
+        <v>7864</v>
+      </c>
+      <c r="F806">
+        <v>16.3</v>
+      </c>
+      <c r="G806" s="3">
+        <v>1031</v>
+      </c>
+      <c r="H806">
+        <v>20.2</v>
+      </c>
+      <c r="I806">
+        <v>376</v>
+      </c>
+      <c r="J806">
+        <v>3.9</v>
+      </c>
+      <c r="K806">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="807" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A807" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B807" t="s">
+        <v>10</v>
+      </c>
+      <c r="C807" t="s">
+        <v>5</v>
+      </c>
+      <c r="D807" s="3">
+        <v>16371</v>
+      </c>
+      <c r="E807" s="3">
+        <v>9955</v>
+      </c>
+      <c r="F807">
+        <v>20.6</v>
+      </c>
+      <c r="G807" s="3">
+        <v>1697</v>
+      </c>
+      <c r="H807">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="I807" s="3">
+        <v>1033</v>
+      </c>
+      <c r="J807">
+        <v>10.7</v>
+      </c>
+      <c r="K807">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="808" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A808" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B808" t="s">
+        <v>10</v>
+      </c>
+      <c r="C808" t="s">
+        <v>6</v>
+      </c>
+      <c r="D808" s="3">
+        <v>16811</v>
+      </c>
+      <c r="E808" s="3">
+        <v>11840</v>
+      </c>
+      <c r="F808">
+        <v>24.5</v>
+      </c>
+      <c r="G808" s="3">
+        <v>1473</v>
+      </c>
+      <c r="H808">
+        <v>28.8</v>
+      </c>
+      <c r="I808" s="3">
+        <v>2843</v>
+      </c>
+      <c r="J808">
+        <v>29.4</v>
+      </c>
+      <c r="K808">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="809" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A809" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B809" t="s">
+        <v>10</v>
+      </c>
+      <c r="C809" t="s">
+        <v>12</v>
+      </c>
+      <c r="D809" s="3">
+        <v>14284</v>
+      </c>
+      <c r="E809" s="3">
+        <v>9038</v>
+      </c>
+      <c r="F809">
+        <v>18.7</v>
+      </c>
+      <c r="G809">
+        <v>172</v>
+      </c>
+      <c r="H809">
+        <v>3.4</v>
+      </c>
+      <c r="I809" s="3">
+        <v>3912</v>
+      </c>
+      <c r="J809">
+        <v>40.5</v>
+      </c>
+      <c r="K809">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="810" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A810" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B810" t="s">
+        <v>10</v>
+      </c>
+      <c r="C810" t="s">
+        <v>13</v>
+      </c>
+      <c r="D810" s="3">
+        <v>4428</v>
+      </c>
+      <c r="E810" s="3">
+        <v>2149</v>
+      </c>
+      <c r="F810">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G810">
+        <v>17</v>
+      </c>
+      <c r="H810">
+        <v>0.3</v>
+      </c>
+      <c r="I810" s="3">
+        <v>1341</v>
+      </c>
+      <c r="J810">
+        <v>13.9</v>
+      </c>
+      <c r="K810">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="811" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A811" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B811" t="s">
+        <v>9</v>
+      </c>
+      <c r="C811" t="s">
+        <v>0</v>
+      </c>
+      <c r="D811">
+        <v>322</v>
+      </c>
+      <c r="E811">
+        <v>103</v>
+      </c>
+      <c r="F811">
+        <v>0.3</v>
+      </c>
+      <c r="G811">
+        <v>11</v>
+      </c>
+      <c r="H811">
+        <v>0.5</v>
+      </c>
+      <c r="I811">
+        <v>1</v>
+      </c>
+      <c r="J811">
+        <v>0</v>
+      </c>
+      <c r="K811">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="812" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A812" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B812" t="s">
+        <v>9</v>
+      </c>
+      <c r="C812" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D812">
+        <v>710</v>
+      </c>
+      <c r="E812">
+        <v>125</v>
+      </c>
+      <c r="F812">
+        <v>0.3</v>
+      </c>
+      <c r="G812">
+        <v>8</v>
+      </c>
+      <c r="H812">
+        <v>0.4</v>
+      </c>
+      <c r="I812">
+        <v>3</v>
+      </c>
+      <c r="J812">
+        <v>0</v>
+      </c>
+      <c r="K812">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="813" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A813" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B813" t="s">
+        <v>9</v>
+      </c>
+      <c r="C813" t="s">
+        <v>1</v>
+      </c>
+      <c r="D813" s="3">
+        <v>7807</v>
+      </c>
+      <c r="E813">
+        <v>707</v>
+      </c>
+      <c r="F813">
+        <v>1.9</v>
+      </c>
+      <c r="G813">
+        <v>37</v>
+      </c>
+      <c r="H813">
+        <v>1.6</v>
+      </c>
+      <c r="I813">
+        <v>8</v>
+      </c>
+      <c r="J813">
+        <v>0.1</v>
+      </c>
+      <c r="K813">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="814" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A814" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B814" t="s">
+        <v>9</v>
+      </c>
+      <c r="C814" t="s">
+        <v>2</v>
+      </c>
+      <c r="D814" s="3">
+        <v>12431</v>
+      </c>
+      <c r="E814" s="3">
+        <v>1675</v>
+      </c>
+      <c r="F814">
+        <v>4.5</v>
+      </c>
+      <c r="G814">
+        <v>93</v>
+      </c>
+      <c r="H814">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I814">
+        <v>22</v>
+      </c>
+      <c r="J814">
+        <v>0.3</v>
+      </c>
+      <c r="K814">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="815" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A815" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B815" t="s">
+        <v>9</v>
+      </c>
+      <c r="C815" t="s">
+        <v>3</v>
+      </c>
+      <c r="D815" s="3">
+        <v>18076</v>
+      </c>
+      <c r="E815" s="3">
+        <v>3385</v>
+      </c>
+      <c r="F815">
+        <v>9.1</v>
+      </c>
+      <c r="G815">
+        <v>219</v>
+      </c>
+      <c r="H815">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I815">
+        <v>64</v>
+      </c>
+      <c r="J815">
+        <v>0.9</v>
+      </c>
+      <c r="K815">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="816" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A816" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B816" t="s">
+        <v>9</v>
+      </c>
+      <c r="C816" t="s">
+        <v>4</v>
+      </c>
+      <c r="D816" s="3">
+        <v>21400</v>
+      </c>
+      <c r="E816" s="3">
+        <v>5381</v>
+      </c>
+      <c r="F816">
+        <v>14.5</v>
+      </c>
+      <c r="G816">
+        <v>423</v>
+      </c>
+      <c r="H816">
+        <v>18.7</v>
+      </c>
+      <c r="I816">
+        <v>151</v>
+      </c>
+      <c r="J816">
+        <v>2.1</v>
+      </c>
+      <c r="K816">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="817" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A817" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B817" t="s">
+        <v>9</v>
+      </c>
+      <c r="C817" t="s">
+        <v>5</v>
+      </c>
+      <c r="D817" s="3">
+        <v>14784</v>
+      </c>
+      <c r="E817" s="3">
+        <v>6484</v>
+      </c>
+      <c r="F817">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G817">
+        <v>662</v>
+      </c>
+      <c r="H817">
+        <v>29.2</v>
+      </c>
+      <c r="I817">
+        <v>426</v>
+      </c>
+      <c r="J817">
+        <v>6</v>
+      </c>
+      <c r="K817">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="818" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A818" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B818" t="s">
+        <v>9</v>
+      </c>
+      <c r="C818" t="s">
+        <v>6</v>
+      </c>
+      <c r="D818" s="3">
+        <v>13332</v>
+      </c>
+      <c r="E818" s="3">
+        <v>7942</v>
+      </c>
+      <c r="F818">
+        <v>21.3</v>
+      </c>
+      <c r="G818">
+        <v>647</v>
+      </c>
+      <c r="H818">
+        <v>28.6</v>
+      </c>
+      <c r="I818" s="3">
+        <v>1318</v>
+      </c>
+      <c r="J818">
+        <v>18.7</v>
+      </c>
+      <c r="K818">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="819" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A819" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B819" t="s">
+        <v>9</v>
+      </c>
+      <c r="C819" t="s">
+        <v>12</v>
+      </c>
+      <c r="D819" s="3">
+        <v>19043</v>
+      </c>
+      <c r="E819" s="3">
+        <v>8140</v>
+      </c>
+      <c r="F819">
+        <v>21.9</v>
+      </c>
+      <c r="G819">
+        <v>140</v>
+      </c>
+      <c r="H819">
+        <v>6.2</v>
+      </c>
+      <c r="I819" s="3">
+        <v>3028</v>
+      </c>
+      <c r="J819">
+        <v>43</v>
+      </c>
+      <c r="K819">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="820" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A820" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B820" t="s">
+        <v>9</v>
+      </c>
+      <c r="C820" t="s">
+        <v>13</v>
+      </c>
+      <c r="D820" s="3">
+        <v>11061</v>
+      </c>
+      <c r="E820" s="3">
+        <v>3294</v>
+      </c>
+      <c r="F820">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G820">
+        <v>26</v>
+      </c>
+      <c r="H820">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I820" s="3">
+        <v>2028</v>
+      </c>
+      <c r="J820">
+        <v>28.8</v>
+      </c>
+      <c r="K820">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="821" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A821" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B821" t="s">
+        <v>10</v>
+      </c>
+      <c r="C821" t="s">
+        <v>0</v>
+      </c>
+      <c r="D821">
+        <v>383</v>
+      </c>
+      <c r="E821">
+        <v>132</v>
+      </c>
+      <c r="F821">
+        <v>0.3</v>
+      </c>
+      <c r="G821">
+        <v>21</v>
+      </c>
+      <c r="H821">
+        <v>0.4</v>
+      </c>
+      <c r="I821">
+        <v>1</v>
+      </c>
+      <c r="J821">
+        <v>0</v>
+      </c>
+      <c r="K821">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="822" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A822" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B822" t="s">
+        <v>10</v>
+      </c>
+      <c r="C822" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D822">
+        <v>572</v>
+      </c>
+      <c r="E822">
+        <v>118</v>
+      </c>
+      <c r="F822">
+        <v>0.2</v>
+      </c>
+      <c r="G822">
+        <v>11</v>
+      </c>
+      <c r="H822">
+        <v>0.2</v>
+      </c>
+      <c r="I822">
+        <v>2</v>
+      </c>
+      <c r="J822">
+        <v>0</v>
+      </c>
+      <c r="K822">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="823" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A823" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B823" t="s">
+        <v>10</v>
+      </c>
+      <c r="C823" t="s">
+        <v>1</v>
+      </c>
+      <c r="D823" s="3">
+        <v>3856</v>
+      </c>
+      <c r="E823">
+        <v>645</v>
+      </c>
+      <c r="F823">
+        <v>1.3</v>
+      </c>
+      <c r="G823">
+        <v>49</v>
+      </c>
+      <c r="H823">
+        <v>1</v>
+      </c>
+      <c r="I823">
+        <v>14</v>
+      </c>
+      <c r="J823">
+        <v>0.1</v>
+      </c>
+      <c r="K823">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="824" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A824" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B824" t="s">
+        <v>10</v>
+      </c>
+      <c r="C824" t="s">
+        <v>2</v>
+      </c>
+      <c r="D824" s="3">
+        <v>7342</v>
+      </c>
+      <c r="E824" s="3">
+        <v>1806</v>
+      </c>
+      <c r="F824">
+        <v>3.7</v>
+      </c>
+      <c r="G824">
+        <v>158</v>
+      </c>
+      <c r="H824">
+        <v>3.1</v>
+      </c>
+      <c r="I824">
+        <v>34</v>
+      </c>
+      <c r="J824">
+        <v>0.4</v>
+      </c>
+      <c r="K824">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="825" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A825" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B825" t="s">
+        <v>10</v>
+      </c>
+      <c r="C825" t="s">
+        <v>3</v>
+      </c>
+      <c r="D825" s="3">
+        <v>12784</v>
+      </c>
+      <c r="E825" s="3">
+        <v>4773</v>
+      </c>
+      <c r="F825">
+        <v>9.9</v>
+      </c>
+      <c r="G825">
+        <v>485</v>
+      </c>
+      <c r="H825">
+        <v>9.5</v>
+      </c>
+      <c r="I825">
+        <v>111</v>
+      </c>
+      <c r="J825">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K825">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="826" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A826" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B826" t="s">
+        <v>10</v>
+      </c>
+      <c r="C826" t="s">
+        <v>4</v>
+      </c>
+      <c r="D826" s="3">
+        <v>16536</v>
+      </c>
+      <c r="E826" s="3">
+        <v>7876</v>
+      </c>
+      <c r="F826">
+        <v>16.3</v>
+      </c>
+      <c r="G826" s="3">
+        <v>1033</v>
+      </c>
+      <c r="H826">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I826">
+        <v>377</v>
+      </c>
+      <c r="J826">
+        <v>3.9</v>
+      </c>
+      <c r="K826">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="827" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A827" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B827" t="s">
+        <v>10</v>
+      </c>
+      <c r="C827" t="s">
+        <v>5</v>
+      </c>
+      <c r="D827" s="3">
+        <v>16441</v>
+      </c>
+      <c r="E827" s="3">
+        <v>9984</v>
+      </c>
+      <c r="F827">
+        <v>20.6</v>
+      </c>
+      <c r="G827" s="3">
+        <v>1705</v>
+      </c>
+      <c r="H827">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="I827" s="3">
+        <v>1035</v>
+      </c>
+      <c r="J827">
+        <v>10.7</v>
+      </c>
+      <c r="K827">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="828" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A828" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B828" t="s">
+        <v>10</v>
+      </c>
+      <c r="C828" t="s">
+        <v>6</v>
+      </c>
+      <c r="D828" s="3">
+        <v>16857</v>
+      </c>
+      <c r="E828" s="3">
+        <v>11863</v>
+      </c>
+      <c r="F828">
+        <v>24.5</v>
+      </c>
+      <c r="G828" s="3">
+        <v>1479</v>
+      </c>
+      <c r="H828">
+        <v>28.8</v>
+      </c>
+      <c r="I828" s="3">
+        <v>2849</v>
+      </c>
+      <c r="J828">
+        <v>29.4</v>
+      </c>
+      <c r="K828">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="829" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A829" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B829" t="s">
+        <v>10</v>
+      </c>
+      <c r="C829" t="s">
+        <v>12</v>
+      </c>
+      <c r="D829" s="3">
+        <v>14305</v>
+      </c>
+      <c r="E829" s="3">
+        <v>9049</v>
+      </c>
+      <c r="F829">
+        <v>18.7</v>
+      </c>
+      <c r="G829">
+        <v>172</v>
+      </c>
+      <c r="H829">
+        <v>3.4</v>
+      </c>
+      <c r="I829" s="3">
+        <v>3918</v>
+      </c>
+      <c r="J829">
+        <v>40.4</v>
+      </c>
+      <c r="K829">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="830" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A830" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B830" t="s">
+        <v>10</v>
+      </c>
+      <c r="C830" t="s">
+        <v>13</v>
+      </c>
+      <c r="D830" s="3">
+        <v>4442</v>
+      </c>
+      <c r="E830" s="3">
+        <v>2155</v>
+      </c>
+      <c r="F830">
+        <v>4.5</v>
+      </c>
+      <c r="G830">
+        <v>18</v>
+      </c>
+      <c r="H830">
+        <v>0.4</v>
+      </c>
+      <c r="I830" s="3">
+        <v>1351</v>
+      </c>
+      <c r="J830">
+        <v>13.9</v>
+      </c>
+      <c r="K830">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="831" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A831" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B831" t="s">
+        <v>9</v>
+      </c>
+      <c r="C831" t="s">
+        <v>0</v>
+      </c>
+      <c r="D831">
+        <v>329</v>
+      </c>
+      <c r="E831">
+        <v>107</v>
+      </c>
+      <c r="F831">
+        <v>0.3</v>
+      </c>
+      <c r="G831">
+        <v>13</v>
+      </c>
+      <c r="H831">
+        <v>0.6</v>
+      </c>
+      <c r="I831">
+        <v>1</v>
+      </c>
+      <c r="J831">
+        <v>0</v>
+      </c>
+      <c r="K831">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="832" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A832" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B832" t="s">
+        <v>9</v>
+      </c>
+      <c r="C832" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D832">
+        <v>726</v>
+      </c>
+      <c r="E832">
+        <v>131</v>
+      </c>
+      <c r="F832">
+        <v>0.3</v>
+      </c>
+      <c r="G832">
+        <v>8</v>
+      </c>
+      <c r="H832">
+        <v>0.3</v>
+      </c>
+      <c r="I832">
+        <v>3</v>
+      </c>
+      <c r="J832">
+        <v>0</v>
+      </c>
+      <c r="K832">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="833" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A833" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B833" t="s">
+        <v>9</v>
+      </c>
+      <c r="C833" t="s">
+        <v>1</v>
+      </c>
+      <c r="D833" s="3">
+        <v>7998</v>
+      </c>
+      <c r="E833">
+        <v>725</v>
+      </c>
+      <c r="F833">
+        <v>1.9</v>
+      </c>
+      <c r="G833">
+        <v>38</v>
+      </c>
+      <c r="H833">
+        <v>1.6</v>
+      </c>
+      <c r="I833">
+        <v>8</v>
+      </c>
+      <c r="J833">
+        <v>0.1</v>
+      </c>
+      <c r="K833">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="834" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A834" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B834" t="s">
+        <v>9</v>
+      </c>
+      <c r="C834" t="s">
+        <v>2</v>
+      </c>
+      <c r="D834" s="3">
+        <v>12666</v>
+      </c>
+      <c r="E834" s="3">
+        <v>1724</v>
+      </c>
+      <c r="F834">
+        <v>4.5</v>
+      </c>
+      <c r="G834">
+        <v>94</v>
+      </c>
+      <c r="H834">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I834">
+        <v>22</v>
+      </c>
+      <c r="J834">
+        <v>0.3</v>
+      </c>
+      <c r="K834">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="835" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A835" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B835" t="s">
+        <v>9</v>
+      </c>
+      <c r="C835" t="s">
+        <v>3</v>
+      </c>
+      <c r="D835" s="3">
+        <v>18407</v>
+      </c>
+      <c r="E835" s="3">
+        <v>3448</v>
+      </c>
+      <c r="F835">
+        <v>9</v>
+      </c>
+      <c r="G835">
+        <v>222</v>
+      </c>
+      <c r="H835">
+        <v>9.6</v>
+      </c>
+      <c r="I835">
+        <v>69</v>
+      </c>
+      <c r="J835">
+        <v>1</v>
+      </c>
+      <c r="K835">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="836" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A836" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B836" t="s">
+        <v>9</v>
+      </c>
+      <c r="C836" t="s">
+        <v>4</v>
+      </c>
+      <c r="D836" s="3">
+        <v>21734</v>
+      </c>
+      <c r="E836" s="3">
+        <v>5515</v>
+      </c>
+      <c r="F836">
+        <v>14.5</v>
+      </c>
+      <c r="G836">
+        <v>431</v>
+      </c>
+      <c r="H836">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I836">
+        <v>160</v>
+      </c>
+      <c r="J836">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K836">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="837" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A837" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B837" t="s">
+        <v>9</v>
+      </c>
+      <c r="C837" t="s">
+        <v>5</v>
+      </c>
+      <c r="D837" s="3">
+        <v>14952</v>
+      </c>
+      <c r="E837" s="3">
+        <v>6580</v>
+      </c>
+      <c r="F837">
+        <v>17.3</v>
+      </c>
+      <c r="G837">
+        <v>678</v>
+      </c>
+      <c r="H837">
+        <v>29.3</v>
+      </c>
+      <c r="I837">
+        <v>438</v>
+      </c>
+      <c r="J837">
+        <v>6.1</v>
+      </c>
+      <c r="K837">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="838" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A838" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B838" t="s">
+        <v>9</v>
+      </c>
+      <c r="C838" t="s">
+        <v>6</v>
+      </c>
+      <c r="D838" s="3">
+        <v>13481</v>
+      </c>
+      <c r="E838" s="3">
+        <v>8081</v>
+      </c>
+      <c r="F838">
+        <v>21.2</v>
+      </c>
+      <c r="G838">
+        <v>661</v>
+      </c>
+      <c r="H838">
+        <v>28.6</v>
+      </c>
+      <c r="I838" s="3">
+        <v>1349</v>
+      </c>
+      <c r="J838">
+        <v>18.7</v>
+      </c>
+      <c r="K838">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="839" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A839" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B839" t="s">
+        <v>9</v>
+      </c>
+      <c r="C839" t="s">
+        <v>12</v>
+      </c>
+      <c r="D839" s="3">
+        <v>19383</v>
+      </c>
+      <c r="E839" s="3">
+        <v>8360</v>
+      </c>
+      <c r="F839">
+        <v>21.9</v>
+      </c>
+      <c r="G839">
+        <v>140</v>
+      </c>
+      <c r="H839">
+        <v>6.1</v>
+      </c>
+      <c r="I839" s="3">
+        <v>3084</v>
+      </c>
+      <c r="J839">
+        <v>42.7</v>
+      </c>
+      <c r="K839">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="840" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A840" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B840" t="s">
+        <v>9</v>
+      </c>
+      <c r="C840" t="s">
+        <v>13</v>
+      </c>
+      <c r="D840" s="3">
+        <v>11309</v>
+      </c>
+      <c r="E840" s="3">
+        <v>3437</v>
+      </c>
+      <c r="F840">
+        <v>9</v>
+      </c>
+      <c r="G840">
+        <v>26</v>
+      </c>
+      <c r="H840">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I840" s="3">
+        <v>2089</v>
+      </c>
+      <c r="J840">
+        <v>28.9</v>
+      </c>
+      <c r="K840">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="841" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A841" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B841" t="s">
+        <v>10</v>
+      </c>
+      <c r="C841" t="s">
+        <v>0</v>
+      </c>
+      <c r="D841">
+        <v>396</v>
+      </c>
+      <c r="E841">
+        <v>139</v>
+      </c>
+      <c r="F841">
+        <v>0.3</v>
+      </c>
+      <c r="G841">
+        <v>24</v>
+      </c>
+      <c r="H841">
+        <v>0.5</v>
+      </c>
+      <c r="I841">
+        <v>1</v>
+      </c>
+      <c r="J841">
+        <v>0</v>
+      </c>
+      <c r="K841">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="842" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A842" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B842" t="s">
+        <v>10</v>
+      </c>
+      <c r="C842" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D842">
+        <v>580</v>
+      </c>
+      <c r="E842">
+        <v>123</v>
+      </c>
+      <c r="F842">
+        <v>0.3</v>
+      </c>
+      <c r="G842">
+        <v>11</v>
+      </c>
+      <c r="H842">
+        <v>0.2</v>
+      </c>
+      <c r="I842">
+        <v>2</v>
+      </c>
+      <c r="J842">
+        <v>0</v>
+      </c>
+      <c r="K842">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="843" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A843" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B843" t="s">
+        <v>10</v>
+      </c>
+      <c r="C843" t="s">
+        <v>1</v>
+      </c>
+      <c r="D843" s="3">
+        <v>3916</v>
+      </c>
+      <c r="E843">
+        <v>655</v>
+      </c>
+      <c r="F843">
+        <v>1.3</v>
+      </c>
+      <c r="G843">
+        <v>49</v>
+      </c>
+      <c r="H843">
+        <v>0.9</v>
+      </c>
+      <c r="I843">
+        <v>14</v>
+      </c>
+      <c r="J843">
+        <v>0.1</v>
+      </c>
+      <c r="K843">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="844" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A844" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B844" t="s">
+        <v>10</v>
+      </c>
+      <c r="C844" t="s">
+        <v>2</v>
+      </c>
+      <c r="D844" s="3">
+        <v>7459</v>
+      </c>
+      <c r="E844" s="3">
+        <v>1851</v>
+      </c>
+      <c r="F844">
+        <v>3.8</v>
+      </c>
+      <c r="G844">
+        <v>162</v>
+      </c>
+      <c r="H844">
+        <v>3.1</v>
+      </c>
+      <c r="I844">
+        <v>35</v>
+      </c>
+      <c r="J844">
+        <v>0.4</v>
+      </c>
+      <c r="K844">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="845" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A845" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B845" t="s">
+        <v>10</v>
+      </c>
+      <c r="C845" t="s">
+        <v>3</v>
+      </c>
+      <c r="D845" s="3">
+        <v>12934</v>
+      </c>
+      <c r="E845" s="3">
+        <v>4852</v>
+      </c>
+      <c r="F845">
+        <v>9.9</v>
+      </c>
+      <c r="G845">
+        <v>494</v>
+      </c>
+      <c r="H845">
+        <v>9.4</v>
+      </c>
+      <c r="I845">
+        <v>113</v>
+      </c>
+      <c r="J845">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K845">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="846" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A846" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B846" t="s">
+        <v>10</v>
+      </c>
+      <c r="C846" t="s">
+        <v>4</v>
+      </c>
+      <c r="D846" s="3">
+        <v>16704</v>
+      </c>
+      <c r="E846" s="3">
+        <v>8016</v>
+      </c>
+      <c r="F846">
+        <v>16.3</v>
+      </c>
+      <c r="G846" s="3">
+        <v>1060</v>
+      </c>
+      <c r="H846">
+        <v>20.3</v>
+      </c>
+      <c r="I846">
+        <v>404</v>
+      </c>
+      <c r="J846">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K846">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="847" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A847" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B847" t="s">
+        <v>10</v>
+      </c>
+      <c r="C847" t="s">
+        <v>5</v>
+      </c>
+      <c r="D847" s="3">
+        <v>16621</v>
+      </c>
+      <c r="E847" s="3">
+        <v>10116</v>
+      </c>
+      <c r="F847">
+        <v>20.6</v>
+      </c>
+      <c r="G847" s="3">
+        <v>1742</v>
+      </c>
+      <c r="H847">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I847" s="3">
+        <v>1077</v>
+      </c>
+      <c r="J847">
+        <v>10.9</v>
+      </c>
+      <c r="K847">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="848" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A848" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B848" t="s">
+        <v>10</v>
+      </c>
+      <c r="C848" t="s">
+        <v>6</v>
+      </c>
+      <c r="D848" s="3">
+        <v>16996</v>
+      </c>
+      <c r="E848" s="3">
+        <v>12004</v>
+      </c>
+      <c r="F848">
+        <v>24.4</v>
+      </c>
+      <c r="G848" s="3">
+        <v>1498</v>
+      </c>
+      <c r="H848">
+        <v>28.6</v>
+      </c>
+      <c r="I848" s="3">
+        <v>2900</v>
+      </c>
+      <c r="J848">
+        <v>29.2</v>
+      </c>
+      <c r="K848">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="849" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A849" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B849" t="s">
+        <v>10</v>
+      </c>
+      <c r="C849" t="s">
+        <v>12</v>
+      </c>
+      <c r="D849" s="3">
+        <v>14453</v>
+      </c>
+      <c r="E849" s="3">
+        <v>9194</v>
+      </c>
+      <c r="F849">
+        <v>18.7</v>
+      </c>
+      <c r="G849">
+        <v>173</v>
+      </c>
+      <c r="H849">
+        <v>3.3</v>
+      </c>
+      <c r="I849" s="3">
+        <v>3987</v>
+      </c>
+      <c r="J849">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="K849">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="850" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A850" s="2">
+        <v>43953</v>
+      </c>
+      <c r="B850" t="s">
+        <v>10</v>
+      </c>
+      <c r="C850" t="s">
+        <v>13</v>
+      </c>
+      <c r="D850" s="3">
+        <v>4519</v>
+      </c>
+      <c r="E850" s="3">
+        <v>2233</v>
+      </c>
+      <c r="F850">
+        <v>4.5</v>
+      </c>
+      <c r="G850">
+        <v>20</v>
+      </c>
+      <c r="H850">
+        <v>0.4</v>
+      </c>
+      <c r="I850" s="3">
+        <v>1383</v>
+      </c>
+      <c r="J850">
+        <v>13.9</v>
+      </c>
+      <c r="K850">
+        <v>30.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding 3-may data and modifications in model, to separate Madrid, La Rioja and Pais Vasco from others
</commit_message>
<xml_diff>
--- a/data/Covid-19_data_sexage.xlsx
+++ b/data/Covid-19_data_sexage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6DCA5-BCF7-DB48-B4B1-3369AE7F866D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF21AB-E9C6-FA4D-9AC7-108DF5AB9605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C24317C9-D1BD-7248-BEC1-07839536F6EA}"/>
   </bookViews>
@@ -60,6 +60,7 @@
     <definedName name="tabula_Actualizacion_92_COVID_19" localSheetId="0">Data!$C$791:$K$810</definedName>
     <definedName name="tabula_Actualizacion_93_COVID_19" localSheetId="0">Data!$C$811:$K$830</definedName>
     <definedName name="tabula_Actualizacion_94_COVID_19" localSheetId="0">Data!$C$831:$K$850</definedName>
+    <definedName name="tabula_Actualizacion_95_COVID_19" localSheetId="0">Data!$C$851:$K$870</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -633,7 +634,7 @@
     </textPr>
   </connection>
   <connection id="38" xr16:uid="{C3E1A69F-8B7E-6B43-BC5D-E06982B30200}" name="tabula-Actualizacion_89_COVID-191" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_89_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_89_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -648,7 +649,7 @@
     </textPr>
   </connection>
   <connection id="39" xr16:uid="{087DFE1B-3741-FE4C-9B0D-327F1CED87AC}" name="tabula-Actualizacion_90_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_90_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_90_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -663,7 +664,7 @@
     </textPr>
   </connection>
   <connection id="40" xr16:uid="{73C49DD9-FD9B-E141-A3F9-FED657D452BB}" name="tabula-Actualizacion_91_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_91_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_91_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -678,7 +679,7 @@
     </textPr>
   </connection>
   <connection id="41" xr16:uid="{976AE8FA-AD7F-D745-A59B-524FC52002A8}" name="tabula-Actualizacion_92_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_92_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_92_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -693,7 +694,7 @@
     </textPr>
   </connection>
   <connection id="42" xr16:uid="{D302820C-066C-364B-BDBB-65072DCE5142}" name="tabula-Actualizacion_93_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_93_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_93_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -708,7 +709,22 @@
     </textPr>
   </connection>
   <connection id="43" xr16:uid="{7D726A8B-9669-2243-9E73-5A200DDE1F7F}" name="tabula-Actualizacion_94_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_94_COVID-19.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_94_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="44" xr16:uid="{B59C3CA5-D7F0-3E4A-B3B5-7C462F22B488}" name="tabula-Actualizacion_95_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_95_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -726,7 +742,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="26">
   <si>
     <t>0-9</t>
   </si>
@@ -904,19 +920,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_94_COVID-19" connectionId="43" xr16:uid="{E1DB3760-CEAD-1243-B89B-5083F9C5FD9D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_95_COVID-19" connectionId="44" xr16:uid="{50535D0C-F452-CC4F-B0B4-D5BD9D462B85}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_80_COVID-19(2)" connectionId="29" xr16:uid="{9A2F5700-61ED-F044-A56E-7B5EC6DF1036}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -924,15 +940,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_84_COVID-19(2)" connectionId="33" xr16:uid="{658D76C0-0942-AF43-952E-435C4A2BDAC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
@@ -940,139 +956,143 @@
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_67_COVID-19(1)" connectionId="16" xr16:uid="{0DCC7075-52E5-6445-A2D9-0D0404D0E63E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_66_COVID-19(1)" connectionId="15" xr16:uid="{784FDDA9-F525-C54F-BA21-682143B55347}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_92_COVID-19" connectionId="41" xr16:uid="{36511222-D462-6C49-8765-A7C39A844257}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_86_COVID-19(2)" connectionId="35" xr16:uid="{95015227-8A0A-4C48-AC40-AEF4A2B2143A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_83_COVID-19(2)" connectionId="32" xr16:uid="{F68CD602-B2A0-604F-A4DC-A153B85916C5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_85_COVID-19(2)" connectionId="34" xr16:uid="{4236AA15-44DD-864C-BBB9-D1CF1013BE00}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_68_COVID-19(1)" connectionId="17" xr16:uid="{15D6F25C-3F4D-0947-8994-7F669D041C1F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_91_COVID-19" connectionId="40" xr16:uid="{84536095-CC54-8C41-83F7-F36B6B61C343}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_81_COVID-19(2)_1" connectionId="30" xr16:uid="{6EBD5E78-C6DF-2E41-9BEC-F2E99D2C6A50}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_79_COVID-19(2)" connectionId="28" xr16:uid="{CE4041F5-2CDB-234C-8611-179139CF531A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="3" xr16:uid="{E94F4815-0D2F-454F-8291-FCBF0C165C57}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_77_COVID-19(2)" connectionId="26" xr16:uid="{B46FF584-84EC-AE4D-BCE8-171BFEBEEDEE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="4" xr16:uid="{10575DCA-3AE8-5C4C-A970-60205B471337}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_90_COVID-19" connectionId="39" xr16:uid="{A93A93AC-3885-8E4E-8C26-49BA468F1F08}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_78_COVID-19(2)" connectionId="27" xr16:uid="{DA1E7C1F-5CE0-764E-9BAE-85540697E15C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_84_COVID-19(2)" connectionId="33" xr16:uid="{658D76C0-0942-AF43-952E-435C4A2BDAC3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_82_COVID-19(2)" connectionId="31" xr16:uid="{0C41A9C7-F783-5441-AFC3-59C34E6567FF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_80_COVID-19(2)" connectionId="29" xr16:uid="{9A2F5700-61ED-F044-A56E-7B5EC6DF1036}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_89_COVID-19" connectionId="38" xr16:uid="{7196C996-97E2-574F-AA83-DA40EB48943E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_94_COVID-19" connectionId="43" xr16:uid="{E1DB3760-CEAD-1243-B89B-5083F9C5FD9D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_93_COVID-19" connectionId="42" xr16:uid="{9B502165-113E-5343-9630-B2499685DBE0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_69_COVID-19(1)" connectionId="18" xr16:uid="{43D60223-767A-964E-8CC2-E64E5ACAFF9F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_88_COVID-19(2)" connectionId="37" xr16:uid="{442A7796-311C-914C-842C-C67D04E6CDF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_85_COVID-19(2)" connectionId="34" xr16:uid="{4236AA15-44DD-864C-BBB9-D1CF1013BE00}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_75_COVID-19(1)" connectionId="24" xr16:uid="{D7A38836-E0C5-5046-B8FD-EF82AA804006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_82_COVID-19(2)" connectionId="31" xr16:uid="{0C41A9C7-F783-5441-AFC3-59C34E6567FF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_53_COVID-19" connectionId="2" xr16:uid="{31483431-2B39-A440-9E59-C26E082912EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_64_COVID-19(1)" connectionId="13" xr16:uid="{24F5186E-14BA-4941-BB1A-F21AEE9F7F07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(2)_1" connectionId="10" xr16:uid="{252D0C3F-8429-6D40-AFE6-2BAFDCF71E62}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_56_COVID-19(1)" connectionId="5" xr16:uid="{C5B10145-DA18-EE44-A918-E407BEA443E9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_70_COVID-19(1)" connectionId="19" xr16:uid="{F30EDCDD-4769-4442-A6A9-407F59F6429F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_92_COVID-19" connectionId="41" xr16:uid="{36511222-D462-6C49-8765-A7C39A844257}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_83_COVID-19(2)" connectionId="32" xr16:uid="{F68CD602-B2A0-604F-A4DC-A153B85916C5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_81_COVID-19(2)_1" connectionId="30" xr16:uid="{6EBD5E78-C6DF-2E41-9BEC-F2E99D2C6A50}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_74_COVID-19(1)" connectionId="23" xr16:uid="{486A1335-E13C-A646-B386-9ED2A72BEEE6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_71_COVID-19(1)" connectionId="20" xr16:uid="{E40B0E49-9F2B-2549-8124-9C24FFB9F4B1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_57_COVID-19(1)" connectionId="6" xr16:uid="{78E004BB-228B-5143-9AFE-91688C440A41}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_73_COVID-19(1)" connectionId="22" xr16:uid="{144BDA4A-6CCF-094D-8B47-C4994B28C9F4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_77_COVID-19(2)" connectionId="26" xr16:uid="{B46FF584-84EC-AE4D-BCE8-171BFEBEEDEE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19(1)" connectionId="9" xr16:uid="{C813FA0B-4B7A-0743-B527-E10C07F0E6C8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_60_COVID-19(1)" connectionId="8" xr16:uid="{C2F0088C-0355-9A48-BE55-175198337C67}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_76_COVID-19(2)" connectionId="25" xr16:uid="{70AE20FA-7C65-AC4F-B077-971D1C6A5B94}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_91_COVID-19" connectionId="40" xr16:uid="{84536095-CC54-8C41-83F7-F36B6B61C343}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_78_COVID-19(2)" connectionId="27" xr16:uid="{DA1E7C1F-5CE0-764E-9BAE-85540697E15C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_62_COVID-19(1)" connectionId="11" xr16:uid="{789174F4-7737-BE4C-9685-F15607B8C828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_72_COVID-19(1)" connectionId="21" xr16:uid="{1488C0E5-7AB9-C44D-8BE2-997243B88982}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_52_COVID-19" connectionId="1" xr16:uid="{35D81D28-1058-4347-9DE2-5F2763DAC2A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_90_COVID-19" connectionId="39" xr16:uid="{A93A93AC-3885-8E4E-8C26-49BA468F1F08}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_89_COVID-19" connectionId="38" xr16:uid="{7196C996-97E2-574F-AA83-DA40EB48943E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_88_COVID-19(2)" connectionId="37" xr16:uid="{442A7796-311C-914C-842C-C67D04E6CDF2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_86_COVID-19(2)" connectionId="35" xr16:uid="{95015227-8A0A-4C48-AC40-AEF4A2B2143A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_59_COVID-19(1)" connectionId="7" xr16:uid="{6E93CE4F-1115-D449-959A-2A7263C31ABC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_63_COVID-19(1)" connectionId="12" xr16:uid="{EFDFC980-4B86-C948-B035-B2786B80754E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1372,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FFFC2-62D5-A048-8409-BF1FADA21B40}">
-  <dimension ref="A1:T850"/>
+  <dimension ref="A1:T870"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A814" workbookViewId="0">
-      <selection activeCell="C842" sqref="C842"/>
+    <sheetView tabSelected="1" topLeftCell="A835" workbookViewId="0">
+      <selection activeCell="B870" sqref="B870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31209,6 +31229,706 @@
         <v>30.6</v>
       </c>
     </row>
+    <row r="851" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A851" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B851" t="s">
+        <v>9</v>
+      </c>
+      <c r="C851" t="s">
+        <v>0</v>
+      </c>
+      <c r="D851">
+        <v>330</v>
+      </c>
+      <c r="E851">
+        <v>107</v>
+      </c>
+      <c r="F851">
+        <v>0.3</v>
+      </c>
+      <c r="G851">
+        <v>13</v>
+      </c>
+      <c r="H851">
+        <v>0.6</v>
+      </c>
+      <c r="I851">
+        <v>1</v>
+      </c>
+      <c r="J851">
+        <v>0</v>
+      </c>
+      <c r="K851">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="852" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A852" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B852" t="s">
+        <v>9</v>
+      </c>
+      <c r="C852" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D852">
+        <v>729</v>
+      </c>
+      <c r="E852">
+        <v>131</v>
+      </c>
+      <c r="F852">
+        <v>0.3</v>
+      </c>
+      <c r="G852">
+        <v>8</v>
+      </c>
+      <c r="H852">
+        <v>0.3</v>
+      </c>
+      <c r="I852">
+        <v>3</v>
+      </c>
+      <c r="J852">
+        <v>0</v>
+      </c>
+      <c r="K852">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="853" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A853" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B853" t="s">
+        <v>9</v>
+      </c>
+      <c r="C853" t="s">
+        <v>1</v>
+      </c>
+      <c r="D853" s="3">
+        <v>8069</v>
+      </c>
+      <c r="E853">
+        <v>727</v>
+      </c>
+      <c r="F853">
+        <v>1.9</v>
+      </c>
+      <c r="G853">
+        <v>38</v>
+      </c>
+      <c r="H853">
+        <v>1.6</v>
+      </c>
+      <c r="I853">
+        <v>8</v>
+      </c>
+      <c r="J853">
+        <v>0.1</v>
+      </c>
+      <c r="K853">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="854" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A854" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B854" t="s">
+        <v>9</v>
+      </c>
+      <c r="C854" t="s">
+        <v>2</v>
+      </c>
+      <c r="D854" s="3">
+        <v>12791</v>
+      </c>
+      <c r="E854" s="3">
+        <v>1726</v>
+      </c>
+      <c r="F854">
+        <v>4.5</v>
+      </c>
+      <c r="G854">
+        <v>94</v>
+      </c>
+      <c r="H854">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I854">
+        <v>22</v>
+      </c>
+      <c r="J854">
+        <v>0.3</v>
+      </c>
+      <c r="K854">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="855" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A855" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B855" t="s">
+        <v>9</v>
+      </c>
+      <c r="C855" t="s">
+        <v>3</v>
+      </c>
+      <c r="D855" s="3">
+        <v>18558</v>
+      </c>
+      <c r="E855" s="3">
+        <v>3453</v>
+      </c>
+      <c r="F855">
+        <v>9</v>
+      </c>
+      <c r="G855">
+        <v>223</v>
+      </c>
+      <c r="H855">
+        <v>9.6</v>
+      </c>
+      <c r="I855">
+        <v>70</v>
+      </c>
+      <c r="J855">
+        <v>1</v>
+      </c>
+      <c r="K855">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="856" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A856" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B856" t="s">
+        <v>9</v>
+      </c>
+      <c r="C856" t="s">
+        <v>4</v>
+      </c>
+      <c r="D856" s="3">
+        <v>21932</v>
+      </c>
+      <c r="E856" s="3">
+        <v>5529</v>
+      </c>
+      <c r="F856">
+        <v>14.5</v>
+      </c>
+      <c r="G856">
+        <v>432</v>
+      </c>
+      <c r="H856">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I856">
+        <v>161</v>
+      </c>
+      <c r="J856">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K856">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="857" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A857" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B857" t="s">
+        <v>9</v>
+      </c>
+      <c r="C857" t="s">
+        <v>5</v>
+      </c>
+      <c r="D857" s="3">
+        <v>15069</v>
+      </c>
+      <c r="E857" s="3">
+        <v>6591</v>
+      </c>
+      <c r="F857">
+        <v>17.3</v>
+      </c>
+      <c r="G857">
+        <v>679</v>
+      </c>
+      <c r="H857">
+        <v>29.3</v>
+      </c>
+      <c r="I857">
+        <v>439</v>
+      </c>
+      <c r="J857">
+        <v>6.1</v>
+      </c>
+      <c r="K857">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="858" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A858" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B858" t="s">
+        <v>9</v>
+      </c>
+      <c r="C858" t="s">
+        <v>6</v>
+      </c>
+      <c r="D858" s="3">
+        <v>13537</v>
+      </c>
+      <c r="E858" s="3">
+        <v>8098</v>
+      </c>
+      <c r="F858">
+        <v>21.2</v>
+      </c>
+      <c r="G858">
+        <v>664</v>
+      </c>
+      <c r="H858">
+        <v>28.7</v>
+      </c>
+      <c r="I858" s="3">
+        <v>1352</v>
+      </c>
+      <c r="J858">
+        <v>18.7</v>
+      </c>
+      <c r="K858">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="859" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A859" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B859" t="s">
+        <v>9</v>
+      </c>
+      <c r="C859" t="s">
+        <v>12</v>
+      </c>
+      <c r="D859" s="3">
+        <v>19462</v>
+      </c>
+      <c r="E859" s="3">
+        <v>8375</v>
+      </c>
+      <c r="F859">
+        <v>21.9</v>
+      </c>
+      <c r="G859">
+        <v>140</v>
+      </c>
+      <c r="H859">
+        <v>6</v>
+      </c>
+      <c r="I859" s="3">
+        <v>3089</v>
+      </c>
+      <c r="J859">
+        <v>42.7</v>
+      </c>
+      <c r="K859">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="860" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A860" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B860" t="s">
+        <v>9</v>
+      </c>
+      <c r="C860" t="s">
+        <v>13</v>
+      </c>
+      <c r="D860" s="3">
+        <v>11355</v>
+      </c>
+      <c r="E860" s="3">
+        <v>3446</v>
+      </c>
+      <c r="F860">
+        <v>9</v>
+      </c>
+      <c r="G860">
+        <v>26</v>
+      </c>
+      <c r="H860">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I860" s="3">
+        <v>2093</v>
+      </c>
+      <c r="J860">
+        <v>28.9</v>
+      </c>
+      <c r="K860">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="861" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A861" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B861" t="s">
+        <v>10</v>
+      </c>
+      <c r="C861" t="s">
+        <v>0</v>
+      </c>
+      <c r="D861">
+        <v>401</v>
+      </c>
+      <c r="E861">
+        <v>140</v>
+      </c>
+      <c r="F861">
+        <v>0.3</v>
+      </c>
+      <c r="G861">
+        <v>25</v>
+      </c>
+      <c r="H861">
+        <v>0.5</v>
+      </c>
+      <c r="I861">
+        <v>1</v>
+      </c>
+      <c r="J861">
+        <v>0</v>
+      </c>
+      <c r="K861">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="862" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A862" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B862" t="s">
+        <v>10</v>
+      </c>
+      <c r="C862" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D862">
+        <v>589</v>
+      </c>
+      <c r="E862">
+        <v>123</v>
+      </c>
+      <c r="F862">
+        <v>0.2</v>
+      </c>
+      <c r="G862">
+        <v>11</v>
+      </c>
+      <c r="H862">
+        <v>0.2</v>
+      </c>
+      <c r="I862">
+        <v>2</v>
+      </c>
+      <c r="J862">
+        <v>0</v>
+      </c>
+      <c r="K862">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="863" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A863" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B863" t="s">
+        <v>10</v>
+      </c>
+      <c r="C863" t="s">
+        <v>1</v>
+      </c>
+      <c r="D863" s="3">
+        <v>3953</v>
+      </c>
+      <c r="E863">
+        <v>657</v>
+      </c>
+      <c r="F863">
+        <v>1.3</v>
+      </c>
+      <c r="G863">
+        <v>50</v>
+      </c>
+      <c r="H863">
+        <v>1</v>
+      </c>
+      <c r="I863">
+        <v>14</v>
+      </c>
+      <c r="J863">
+        <v>0.1</v>
+      </c>
+      <c r="K863">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="864" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A864" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B864" t="s">
+        <v>10</v>
+      </c>
+      <c r="C864" t="s">
+        <v>2</v>
+      </c>
+      <c r="D864" s="3">
+        <v>7521</v>
+      </c>
+      <c r="E864" s="3">
+        <v>1852</v>
+      </c>
+      <c r="F864">
+        <v>3.8</v>
+      </c>
+      <c r="G864">
+        <v>162</v>
+      </c>
+      <c r="H864">
+        <v>3.1</v>
+      </c>
+      <c r="I864">
+        <v>35</v>
+      </c>
+      <c r="J864">
+        <v>0.4</v>
+      </c>
+      <c r="K864">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="865" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A865" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B865" t="s">
+        <v>10</v>
+      </c>
+      <c r="C865" t="s">
+        <v>3</v>
+      </c>
+      <c r="D865" s="3">
+        <v>13010</v>
+      </c>
+      <c r="E865" s="3">
+        <v>4859</v>
+      </c>
+      <c r="F865">
+        <v>9.9</v>
+      </c>
+      <c r="G865">
+        <v>495</v>
+      </c>
+      <c r="H865">
+        <v>9.4</v>
+      </c>
+      <c r="I865">
+        <v>113</v>
+      </c>
+      <c r="J865">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K865">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="866" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A866" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B866" t="s">
+        <v>10</v>
+      </c>
+      <c r="C866" t="s">
+        <v>4</v>
+      </c>
+      <c r="D866" s="3">
+        <v>16788</v>
+      </c>
+      <c r="E866" s="3">
+        <v>8029</v>
+      </c>
+      <c r="F866">
+        <v>16.3</v>
+      </c>
+      <c r="G866" s="3">
+        <v>1062</v>
+      </c>
+      <c r="H866">
+        <v>20.3</v>
+      </c>
+      <c r="I866">
+        <v>405</v>
+      </c>
+      <c r="J866">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K866">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="867" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A867" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B867" t="s">
+        <v>10</v>
+      </c>
+      <c r="C867" t="s">
+        <v>5</v>
+      </c>
+      <c r="D867" s="3">
+        <v>16698</v>
+      </c>
+      <c r="E867" s="3">
+        <v>10137</v>
+      </c>
+      <c r="F867">
+        <v>20.6</v>
+      </c>
+      <c r="G867" s="3">
+        <v>1744</v>
+      </c>
+      <c r="H867">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="I867" s="3">
+        <v>1079</v>
+      </c>
+      <c r="J867">
+        <v>10.9</v>
+      </c>
+      <c r="K867">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="868" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A868" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B868" t="s">
+        <v>10</v>
+      </c>
+      <c r="C868" t="s">
+        <v>6</v>
+      </c>
+      <c r="D868" s="3">
+        <v>17046</v>
+      </c>
+      <c r="E868" s="3">
+        <v>12037</v>
+      </c>
+      <c r="F868">
+        <v>24.4</v>
+      </c>
+      <c r="G868" s="3">
+        <v>1502</v>
+      </c>
+      <c r="H868">
+        <v>28.6</v>
+      </c>
+      <c r="I868" s="3">
+        <v>2908</v>
+      </c>
+      <c r="J868">
+        <v>29.3</v>
+      </c>
+      <c r="K868">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="869" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A869" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B869" t="s">
+        <v>10</v>
+      </c>
+      <c r="C869" t="s">
+        <v>12</v>
+      </c>
+      <c r="D869" s="3">
+        <v>14480</v>
+      </c>
+      <c r="E869" s="3">
+        <v>9206</v>
+      </c>
+      <c r="F869">
+        <v>18.7</v>
+      </c>
+      <c r="G869">
+        <v>172</v>
+      </c>
+      <c r="H869">
+        <v>3.3</v>
+      </c>
+      <c r="I869" s="3">
+        <v>3997</v>
+      </c>
+      <c r="J869">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="K869">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="870" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A870" s="2">
+        <v>43954</v>
+      </c>
+      <c r="B870" t="s">
+        <v>10</v>
+      </c>
+      <c r="C870" t="s">
+        <v>13</v>
+      </c>
+      <c r="D870" s="3">
+        <v>4527</v>
+      </c>
+      <c r="E870" s="3">
+        <v>2236</v>
+      </c>
+      <c r="F870">
+        <v>4.5</v>
+      </c>
+      <c r="G870">
+        <v>21</v>
+      </c>
+      <c r="H870">
+        <v>0.4</v>
+      </c>
+      <c r="I870" s="3">
+        <v>1386</v>
+      </c>
+      <c r="J870">
+        <v>13.9</v>
+      </c>
+      <c r="K870">
+        <v>30.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>